<commit_message>
Added event types to Excel file. Added latex table generation to script.
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="60">
   <si>
     <t xml:space="preserve">should_escalate</t>
   </si>
@@ -203,16 +203,20 @@
   <si>
     <t xml:space="preserve">id</t>
   </si>
+  <si>
+    <t xml:space="preserve">True/False alarm</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00%"/>
     <numFmt numFmtId="166" formatCode="0%"/>
     <numFmt numFmtId="167" formatCode="0"/>
+    <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -306,7 +310,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -335,15 +339,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -426,8 +438,8 @@
   </sheetPr>
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A50" activeCellId="0" sqref="A2:A74"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A50" activeCellId="0" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -674,41 +686,41 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="n">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="7" t="n">
+      <c r="C7" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="D7" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="7" t="s">
+      <c r="D7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="7" t="n">
+      <c r="G7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="H7" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="I7" s="7" t="s">
+      <c r="H7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I7" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="7" t="n">
+      <c r="J7" s="0" t="n">
         <v>0.79</v>
       </c>
       <c r="K7" s="6" t="n">
         <v>0.9</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="L7" s="0" t="s">
         <v>20</v>
       </c>
     </row>
@@ -781,7 +793,7 @@
       <c r="J9" s="0" t="n">
         <v>0.95</v>
       </c>
-      <c r="K9" s="8" t="n">
+      <c r="K9" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L9" s="0" t="s">
@@ -819,7 +831,7 @@
       <c r="J10" s="0" t="n">
         <v>1.22</v>
       </c>
-      <c r="K10" s="8" t="n">
+      <c r="K10" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L10" s="0" t="s">
@@ -857,7 +869,7 @@
       <c r="J11" s="0" t="n">
         <v>0.71</v>
       </c>
-      <c r="K11" s="8" t="n">
+      <c r="K11" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L11" s="0" t="s">
@@ -895,7 +907,7 @@
       <c r="J12" s="0" t="n">
         <v>1.3</v>
       </c>
-      <c r="K12" s="8" t="n">
+      <c r="K12" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L12" s="0" t="s">
@@ -933,7 +945,7 @@
       <c r="J13" s="0" t="n">
         <v>0.47</v>
       </c>
-      <c r="K13" s="8" t="n">
+      <c r="K13" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L13" s="0" t="s">
@@ -971,7 +983,7 @@
       <c r="J14" s="0" t="n">
         <v>0.68</v>
       </c>
-      <c r="K14" s="8" t="n">
+      <c r="K14" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L14" s="0" t="s">
@@ -1009,7 +1021,7 @@
       <c r="J15" s="0" t="n">
         <v>1.28</v>
       </c>
-      <c r="K15" s="8" t="n">
+      <c r="K15" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L15" s="0" t="s">
@@ -1047,7 +1059,7 @@
       <c r="J16" s="0" t="n">
         <v>0.37</v>
       </c>
-      <c r="K16" s="8" t="n">
+      <c r="K16" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L16" s="0" t="s">
@@ -1085,7 +1097,7 @@
       <c r="J17" s="0" t="n">
         <v>0.89</v>
       </c>
-      <c r="K17" s="8" t="n">
+      <c r="K17" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L17" s="0" t="s">
@@ -1123,7 +1135,7 @@
       <c r="J18" s="0" t="n">
         <v>1.11</v>
       </c>
-      <c r="K18" s="8" t="n">
+      <c r="K18" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L18" s="0" t="s">
@@ -1161,7 +1173,7 @@
       <c r="J19" s="0" t="n">
         <v>0.9</v>
       </c>
-      <c r="K19" s="8" t="n">
+      <c r="K19" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L19" s="0" t="s">
@@ -1199,7 +1211,7 @@
       <c r="J20" s="0" t="n">
         <v>0.61</v>
       </c>
-      <c r="K20" s="8" t="n">
+      <c r="K20" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L20" s="0" t="s">
@@ -1237,7 +1249,7 @@
       <c r="J21" s="0" t="n">
         <v>0.16</v>
       </c>
-      <c r="K21" s="8" t="n">
+      <c r="K21" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L21" s="0" t="s">
@@ -1275,7 +1287,7 @@
       <c r="J22" s="0" t="n">
         <v>0.09</v>
       </c>
-      <c r="K22" s="8" t="n">
+      <c r="K22" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L22" s="0" t="s">
@@ -1313,10 +1325,10 @@
       <c r="J23" s="0" t="n">
         <v>5.78</v>
       </c>
-      <c r="K23" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L23" s="7" t="s">
+      <c r="K23" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1351,10 +1363,10 @@
       <c r="J24" s="0" t="n">
         <v>5.36</v>
       </c>
-      <c r="K24" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L24" s="7" t="s">
+      <c r="K24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1389,10 +1401,10 @@
       <c r="J25" s="0" t="n">
         <v>2.85</v>
       </c>
-      <c r="K25" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L25" s="7" t="s">
+      <c r="K25" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1427,10 +1439,10 @@
       <c r="J26" s="0" t="n">
         <v>5.53</v>
       </c>
-      <c r="K26" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L26" s="7" t="s">
+      <c r="K26" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1465,10 +1477,10 @@
       <c r="J27" s="0" t="n">
         <v>1.29</v>
       </c>
-      <c r="K27" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L27" s="7" t="s">
+      <c r="K27" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1503,10 +1515,10 @@
       <c r="J28" s="0" t="n">
         <v>2.48</v>
       </c>
-      <c r="K28" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L28" s="7" t="s">
+      <c r="K28" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1541,10 +1553,10 @@
       <c r="J29" s="0" t="n">
         <v>5.65</v>
       </c>
-      <c r="K29" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L29" s="7" t="s">
+      <c r="K29" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L29" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1579,10 +1591,10 @@
       <c r="J30" s="0" t="n">
         <v>2.8</v>
       </c>
-      <c r="K30" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L30" s="7" t="s">
+      <c r="K30" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L30" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1617,10 +1629,10 @@
       <c r="J31" s="0" t="n">
         <v>4.32</v>
       </c>
-      <c r="K31" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L31" s="7" t="s">
+      <c r="K31" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L31" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1655,10 +1667,10 @@
       <c r="J32" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="K32" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L32" s="7" t="s">
+      <c r="K32" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L32" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1693,10 +1705,10 @@
       <c r="J33" s="0" t="n">
         <v>2.53</v>
       </c>
-      <c r="K33" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L33" s="7" t="s">
+      <c r="K33" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L33" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1731,10 +1743,10 @@
       <c r="J34" s="0" t="n">
         <v>4.48</v>
       </c>
-      <c r="K34" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L34" s="7" t="s">
+      <c r="K34" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L34" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1769,10 +1781,10 @@
       <c r="J35" s="0" t="n">
         <v>8.15</v>
       </c>
-      <c r="K35" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L35" s="7" t="s">
+      <c r="K35" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L35" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1807,10 +1819,10 @@
       <c r="J36" s="0" t="n">
         <v>2.97</v>
       </c>
-      <c r="K36" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L36" s="7" t="s">
+      <c r="K36" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L36" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1845,10 +1857,10 @@
       <c r="J37" s="0" t="n">
         <v>4.3</v>
       </c>
-      <c r="K37" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L37" s="7" t="s">
+      <c r="K37" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L37" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1883,7 +1895,7 @@
       <c r="J38" s="0" t="n">
         <v>0.41</v>
       </c>
-      <c r="K38" s="8" t="n">
+      <c r="K38" s="7" t="n">
         <v>0.53</v>
       </c>
       <c r="L38" s="0" t="s">
@@ -1921,7 +1933,7 @@
       <c r="J39" s="0" t="n">
         <v>0.16</v>
       </c>
-      <c r="K39" s="8" t="n">
+      <c r="K39" s="7" t="n">
         <v>0.66</v>
       </c>
       <c r="L39" s="0" t="s">
@@ -1959,7 +1971,7 @@
       <c r="J40" s="0" t="n">
         <v>1.22</v>
       </c>
-      <c r="K40" s="8" t="n">
+      <c r="K40" s="7" t="n">
         <v>0.51</v>
       </c>
       <c r="L40" s="0" t="s">
@@ -1997,7 +2009,7 @@
       <c r="J41" s="0" t="n">
         <v>0.58</v>
       </c>
-      <c r="K41" s="8" t="n">
+      <c r="K41" s="7" t="n">
         <v>0.63</v>
       </c>
       <c r="L41" s="0" t="s">
@@ -2035,7 +2047,7 @@
       <c r="J42" s="0" t="n">
         <v>0.56</v>
       </c>
-      <c r="K42" s="8" t="n">
+      <c r="K42" s="7" t="n">
         <v>0.57</v>
       </c>
       <c r="L42" s="0" t="s">
@@ -2073,7 +2085,7 @@
       <c r="J43" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="K43" s="8" t="n">
+      <c r="K43" s="7" t="n">
         <v>0.69</v>
       </c>
       <c r="L43" s="0" t="s">
@@ -2111,7 +2123,7 @@
       <c r="J44" s="0" t="n">
         <v>1.18</v>
       </c>
-      <c r="K44" s="8" t="n">
+      <c r="K44" s="7" t="n">
         <v>0.71</v>
       </c>
       <c r="L44" s="0" t="s">
@@ -2149,7 +2161,7 @@
       <c r="J45" s="0" t="n">
         <v>0.9</v>
       </c>
-      <c r="K45" s="8" t="n">
+      <c r="K45" s="7" t="n">
         <v>0.71</v>
       </c>
       <c r="L45" s="0" t="s">
@@ -2187,7 +2199,7 @@
       <c r="J46" s="0" t="n">
         <v>1.28</v>
       </c>
-      <c r="K46" s="8" t="n">
+      <c r="K46" s="7" t="n">
         <v>0.55</v>
       </c>
       <c r="L46" s="0" t="s">
@@ -2225,7 +2237,7 @@
       <c r="J47" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K47" s="8" t="n">
+      <c r="K47" s="7" t="n">
         <v>0.55</v>
       </c>
       <c r="L47" s="0" t="s">
@@ -2263,7 +2275,7 @@
       <c r="J48" s="0" t="n">
         <v>0.95</v>
       </c>
-      <c r="K48" s="8" t="n">
+      <c r="K48" s="7" t="n">
         <v>0.69</v>
       </c>
       <c r="L48" s="0" t="s">
@@ -2301,7 +2313,7 @@
       <c r="J49" s="0" t="n">
         <v>0.95</v>
       </c>
-      <c r="K49" s="8" t="n">
+      <c r="K49" s="7" t="n">
         <v>0.69</v>
       </c>
       <c r="L49" s="0" t="s">
@@ -2343,8 +2355,8 @@
   </sheetPr>
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A2:A74"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2431,14 +2443,14 @@
       <c r="J2" s="0" t="n">
         <v>0.15</v>
       </c>
-      <c r="K2" s="8" t="n">
+      <c r="K2" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L2" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="9"/>
-      <c r="P2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -2471,13 +2483,13 @@
       <c r="J3" s="0" t="n">
         <v>1.68</v>
       </c>
-      <c r="K3" s="8" t="n">
+      <c r="K3" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L3" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P3" s="8"/>
+      <c r="P3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -2510,13 +2522,13 @@
       <c r="J4" s="0" t="n">
         <v>1.84</v>
       </c>
-      <c r="K4" s="8" t="n">
+      <c r="K4" s="7" t="n">
         <v>0.28</v>
       </c>
       <c r="L4" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P4" s="8"/>
+      <c r="P4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -2549,13 +2561,13 @@
       <c r="J5" s="0" t="n">
         <v>1.75</v>
       </c>
-      <c r="K5" s="8" t="n">
+      <c r="K5" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L5" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P5" s="8"/>
+      <c r="P5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -2588,13 +2600,13 @@
       <c r="J6" s="0" t="n">
         <v>0.77</v>
       </c>
-      <c r="K6" s="8" t="n">
+      <c r="K6" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L6" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P6" s="8"/>
+      <c r="P6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -2627,13 +2639,13 @@
       <c r="J7" s="0" t="n">
         <v>0.65</v>
       </c>
-      <c r="K7" s="8" t="n">
+      <c r="K7" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L7" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P7" s="8"/>
+      <c r="P7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -2666,13 +2678,13 @@
       <c r="J8" s="0" t="n">
         <v>0.68</v>
       </c>
-      <c r="K8" s="8" t="n">
+      <c r="K8" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L8" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P8" s="8"/>
+      <c r="P8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -2705,13 +2717,13 @@
       <c r="J9" s="0" t="n">
         <v>2.1</v>
       </c>
-      <c r="K9" s="8" t="n">
+      <c r="K9" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L9" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P9" s="8"/>
+      <c r="P9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -2744,13 +2756,13 @@
       <c r="J10" s="0" t="n">
         <v>1.76</v>
       </c>
-      <c r="K10" s="8" t="n">
+      <c r="K10" s="7" t="n">
         <v>0.26</v>
       </c>
       <c r="L10" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P10" s="8"/>
+      <c r="P10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -2783,13 +2795,13 @@
       <c r="J11" s="0" t="n">
         <v>0.05</v>
       </c>
-      <c r="K11" s="8" t="n">
+      <c r="K11" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L11" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P11" s="8"/>
+      <c r="P11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -2822,13 +2834,13 @@
       <c r="J12" s="0" t="n">
         <v>2.43</v>
       </c>
-      <c r="K12" s="8" t="n">
+      <c r="K12" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L12" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P12" s="8"/>
+      <c r="P12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -2861,13 +2873,13 @@
       <c r="J13" s="0" t="n">
         <v>0.34</v>
       </c>
-      <c r="K13" s="8" t="n">
+      <c r="K13" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L13" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P13" s="8"/>
+      <c r="P13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -2900,13 +2912,13 @@
       <c r="J14" s="0" t="n">
         <v>1.75</v>
       </c>
-      <c r="K14" s="8" t="n">
+      <c r="K14" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L14" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P14" s="8"/>
+      <c r="P14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -2939,13 +2951,13 @@
       <c r="J15" s="0" t="n">
         <v>1.75</v>
       </c>
-      <c r="K15" s="8" t="n">
+      <c r="K15" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L15" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P15" s="8"/>
+      <c r="P15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -2978,13 +2990,13 @@
       <c r="J16" s="0" t="n">
         <v>1.44</v>
       </c>
-      <c r="K16" s="8" t="n">
+      <c r="K16" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L16" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P16" s="8"/>
+      <c r="P16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
@@ -3017,13 +3029,13 @@
       <c r="J17" s="0" t="n">
         <v>0.63</v>
       </c>
-      <c r="K17" s="8" t="n">
+      <c r="K17" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L17" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P17" s="8"/>
+      <c r="P17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
@@ -3056,13 +3068,13 @@
       <c r="J18" s="0" t="n">
         <v>2.15</v>
       </c>
-      <c r="K18" s="8" t="n">
+      <c r="K18" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L18" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P18" s="8"/>
+      <c r="P18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
@@ -3095,13 +3107,13 @@
       <c r="J19" s="0" t="n">
         <v>0.32</v>
       </c>
-      <c r="K19" s="8" t="n">
+      <c r="K19" s="7" t="n">
         <v>0.38</v>
       </c>
       <c r="L19" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="P19" s="8"/>
+      <c r="P19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -3134,14 +3146,14 @@
       <c r="J20" s="0" t="n">
         <v>1.65</v>
       </c>
-      <c r="K20" s="8" t="n">
+      <c r="K20" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L20" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="O20" s="9"/>
-      <c r="P20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
@@ -3174,14 +3186,14 @@
       <c r="J21" s="0" t="n">
         <v>0.46</v>
       </c>
-      <c r="K21" s="8" t="n">
+      <c r="K21" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L21" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="O21" s="9"/>
-      <c r="P21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
@@ -3214,14 +3226,14 @@
       <c r="J22" s="0" t="n">
         <v>1.16</v>
       </c>
-      <c r="K22" s="8" t="n">
+      <c r="K22" s="7" t="n">
         <v>0.34</v>
       </c>
       <c r="L22" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="O22" s="9"/>
-      <c r="P22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="7"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -3254,14 +3266,14 @@
       <c r="J23" s="0" t="n">
         <v>1.77</v>
       </c>
-      <c r="K23" s="8" t="n">
+      <c r="K23" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L23" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="O23" s="9"/>
-      <c r="P23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="7"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
@@ -3294,14 +3306,14 @@
       <c r="J24" s="0" t="n">
         <v>1.91</v>
       </c>
-      <c r="K24" s="8" t="n">
+      <c r="K24" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L24" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="O24" s="9"/>
-      <c r="P24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="7"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
@@ -3334,14 +3346,14 @@
       <c r="J25" s="0" t="n">
         <v>0.64</v>
       </c>
-      <c r="K25" s="8" t="n">
+      <c r="K25" s="7" t="n">
         <v>0.36</v>
       </c>
       <c r="L25" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="O25" s="9"/>
-      <c r="P25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="7"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
@@ -3374,14 +3386,14 @@
       <c r="J26" s="0" t="n">
         <v>0.81</v>
       </c>
-      <c r="K26" s="8" t="n">
+      <c r="K26" s="7" t="n">
         <v>0</v>
       </c>
       <c r="L26" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="O26" s="9"/>
-      <c r="P26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3401,8 +3413,8 @@
   </sheetPr>
   <dimension ref="A1:K72"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A74 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3458,7 +3470,7 @@
       <c r="J2" s="0" t="n">
         <v>0.15</v>
       </c>
-      <c r="K2" s="8" t="n">
+      <c r="K2" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3703,7 +3715,7 @@
       <c r="J9" s="0" t="n">
         <v>0.95</v>
       </c>
-      <c r="K9" s="8" t="n">
+      <c r="K9" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3738,7 +3750,7 @@
       <c r="J10" s="0" t="n">
         <v>1.22</v>
       </c>
-      <c r="K10" s="8" t="n">
+      <c r="K10" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3773,7 +3785,7 @@
       <c r="J11" s="0" t="n">
         <v>0.71</v>
       </c>
-      <c r="K11" s="8" t="n">
+      <c r="K11" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3808,7 +3820,7 @@
       <c r="J12" s="0" t="n">
         <v>1.3</v>
       </c>
-      <c r="K12" s="8" t="n">
+      <c r="K12" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3843,7 +3855,7 @@
       <c r="J13" s="0" t="n">
         <v>0.47</v>
       </c>
-      <c r="K13" s="8" t="n">
+      <c r="K13" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3878,7 +3890,7 @@
       <c r="J14" s="0" t="n">
         <v>0.68</v>
       </c>
-      <c r="K14" s="8" t="n">
+      <c r="K14" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3913,7 +3925,7 @@
       <c r="J15" s="0" t="n">
         <v>1.28</v>
       </c>
-      <c r="K15" s="8" t="n">
+      <c r="K15" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3948,7 +3960,7 @@
       <c r="J16" s="0" t="n">
         <v>0.37</v>
       </c>
-      <c r="K16" s="8" t="n">
+      <c r="K16" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3983,7 +3995,7 @@
       <c r="J17" s="0" t="n">
         <v>0.89</v>
       </c>
-      <c r="K17" s="8" t="n">
+      <c r="K17" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4018,7 +4030,7 @@
       <c r="J18" s="0" t="n">
         <v>1.11</v>
       </c>
-      <c r="K18" s="8" t="n">
+      <c r="K18" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4053,7 +4065,7 @@
       <c r="J19" s="0" t="n">
         <v>0.9</v>
       </c>
-      <c r="K19" s="8" t="n">
+      <c r="K19" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4088,7 +4100,7 @@
       <c r="J20" s="0" t="n">
         <v>0.61</v>
       </c>
-      <c r="K20" s="8" t="n">
+      <c r="K20" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4123,7 +4135,7 @@
       <c r="J21" s="0" t="n">
         <v>0.16</v>
       </c>
-      <c r="K21" s="8" t="n">
+      <c r="K21" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4158,7 +4170,7 @@
       <c r="J22" s="0" t="n">
         <v>0.09</v>
       </c>
-      <c r="K22" s="8" t="n">
+      <c r="K22" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4193,7 +4205,7 @@
       <c r="J23" s="0" t="n">
         <v>5.78</v>
       </c>
-      <c r="K23" s="8" t="n">
+      <c r="K23" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4228,7 +4240,7 @@
       <c r="J24" s="0" t="n">
         <v>5.36</v>
       </c>
-      <c r="K24" s="8" t="n">
+      <c r="K24" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4263,7 +4275,7 @@
       <c r="J25" s="0" t="n">
         <v>2.85</v>
       </c>
-      <c r="K25" s="8" t="n">
+      <c r="K25" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4298,7 +4310,7 @@
       <c r="J26" s="0" t="n">
         <v>5.53</v>
       </c>
-      <c r="K26" s="8" t="n">
+      <c r="K26" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4333,7 +4345,7 @@
       <c r="J27" s="0" t="n">
         <v>1.29</v>
       </c>
-      <c r="K27" s="8" t="n">
+      <c r="K27" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4368,7 +4380,7 @@
       <c r="J28" s="0" t="n">
         <v>2.48</v>
       </c>
-      <c r="K28" s="8" t="n">
+      <c r="K28" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4403,7 +4415,7 @@
       <c r="J29" s="0" t="n">
         <v>5.65</v>
       </c>
-      <c r="K29" s="8" t="n">
+      <c r="K29" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4438,7 +4450,7 @@
       <c r="J30" s="0" t="n">
         <v>2.8</v>
       </c>
-      <c r="K30" s="8" t="n">
+      <c r="K30" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4473,7 +4485,7 @@
       <c r="J31" s="0" t="n">
         <v>4.32</v>
       </c>
-      <c r="K31" s="8" t="n">
+      <c r="K31" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4508,7 +4520,7 @@
       <c r="J32" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="K32" s="8" t="n">
+      <c r="K32" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4543,7 +4555,7 @@
       <c r="J33" s="0" t="n">
         <v>2.53</v>
       </c>
-      <c r="K33" s="8" t="n">
+      <c r="K33" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4578,7 +4590,7 @@
       <c r="J34" s="0" t="n">
         <v>4.48</v>
       </c>
-      <c r="K34" s="8" t="n">
+      <c r="K34" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4613,7 +4625,7 @@
       <c r="J35" s="0" t="n">
         <v>8.15</v>
       </c>
-      <c r="K35" s="8" t="n">
+      <c r="K35" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4648,7 +4660,7 @@
       <c r="J36" s="0" t="n">
         <v>2.97</v>
       </c>
-      <c r="K36" s="8" t="n">
+      <c r="K36" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4683,7 +4695,7 @@
       <c r="J37" s="0" t="n">
         <v>4.3</v>
       </c>
-      <c r="K37" s="8" t="n">
+      <c r="K37" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4718,7 +4730,7 @@
       <c r="J38" s="0" t="n">
         <v>0.41</v>
       </c>
-      <c r="K38" s="8" t="n">
+      <c r="K38" s="7" t="n">
         <v>0.53</v>
       </c>
     </row>
@@ -4753,7 +4765,7 @@
       <c r="J39" s="0" t="n">
         <v>0.16</v>
       </c>
-      <c r="K39" s="8" t="n">
+      <c r="K39" s="7" t="n">
         <v>0.66</v>
       </c>
     </row>
@@ -4788,7 +4800,7 @@
       <c r="J40" s="0" t="n">
         <v>1.22</v>
       </c>
-      <c r="K40" s="8" t="n">
+      <c r="K40" s="7" t="n">
         <v>0.51</v>
       </c>
     </row>
@@ -4823,7 +4835,7 @@
       <c r="J41" s="0" t="n">
         <v>0.58</v>
       </c>
-      <c r="K41" s="8" t="n">
+      <c r="K41" s="7" t="n">
         <v>0.63</v>
       </c>
     </row>
@@ -4858,7 +4870,7 @@
       <c r="J42" s="0" t="n">
         <v>0.56</v>
       </c>
-      <c r="K42" s="8" t="n">
+      <c r="K42" s="7" t="n">
         <v>0.57</v>
       </c>
     </row>
@@ -4893,7 +4905,7 @@
       <c r="J43" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="K43" s="8" t="n">
+      <c r="K43" s="7" t="n">
         <v>0.69</v>
       </c>
     </row>
@@ -4928,7 +4940,7 @@
       <c r="J44" s="0" t="n">
         <v>1.18</v>
       </c>
-      <c r="K44" s="8" t="n">
+      <c r="K44" s="7" t="n">
         <v>0.71</v>
       </c>
     </row>
@@ -4963,7 +4975,7 @@
       <c r="J45" s="0" t="n">
         <v>0.9</v>
       </c>
-      <c r="K45" s="8" t="n">
+      <c r="K45" s="7" t="n">
         <v>0.71</v>
       </c>
     </row>
@@ -4998,7 +5010,7 @@
       <c r="J46" s="0" t="n">
         <v>1.28</v>
       </c>
-      <c r="K46" s="8" t="n">
+      <c r="K46" s="7" t="n">
         <v>0.55</v>
       </c>
     </row>
@@ -5033,7 +5045,7 @@
       <c r="J47" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K47" s="8" t="n">
+      <c r="K47" s="7" t="n">
         <v>0.55</v>
       </c>
     </row>
@@ -5068,7 +5080,7 @@
       <c r="J48" s="0" t="n">
         <v>0.95</v>
       </c>
-      <c r="K48" s="8" t="n">
+      <c r="K48" s="7" t="n">
         <v>0.69</v>
       </c>
     </row>
@@ -5103,7 +5115,7 @@
       <c r="J49" s="0" t="n">
         <v>1.68</v>
       </c>
-      <c r="K49" s="8" t="n">
+      <c r="K49" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5138,7 +5150,7 @@
       <c r="J50" s="0" t="n">
         <v>1.84</v>
       </c>
-      <c r="K50" s="8" t="n">
+      <c r="K50" s="7" t="n">
         <v>0.28</v>
       </c>
     </row>
@@ -5173,7 +5185,7 @@
       <c r="J51" s="0" t="n">
         <v>1.75</v>
       </c>
-      <c r="K51" s="8" t="n">
+      <c r="K51" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5208,7 +5220,7 @@
       <c r="J52" s="0" t="n">
         <v>0.77</v>
       </c>
-      <c r="K52" s="8" t="n">
+      <c r="K52" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5243,7 +5255,7 @@
       <c r="J53" s="0" t="n">
         <v>0.65</v>
       </c>
-      <c r="K53" s="8" t="n">
+      <c r="K53" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5278,7 +5290,7 @@
       <c r="J54" s="0" t="n">
         <v>0.68</v>
       </c>
-      <c r="K54" s="8" t="n">
+      <c r="K54" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5313,7 +5325,7 @@
       <c r="J55" s="0" t="n">
         <v>2.1</v>
       </c>
-      <c r="K55" s="8" t="n">
+      <c r="K55" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5348,7 +5360,7 @@
       <c r="J56" s="0" t="n">
         <v>1.76</v>
       </c>
-      <c r="K56" s="8" t="n">
+      <c r="K56" s="7" t="n">
         <v>0.26</v>
       </c>
     </row>
@@ -5383,7 +5395,7 @@
       <c r="J57" s="0" t="n">
         <v>0.05</v>
       </c>
-      <c r="K57" s="8" t="n">
+      <c r="K57" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5418,7 +5430,7 @@
       <c r="J58" s="0" t="n">
         <v>2.43</v>
       </c>
-      <c r="K58" s="8" t="n">
+      <c r="K58" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5453,7 +5465,7 @@
       <c r="J59" s="0" t="n">
         <v>0.34</v>
       </c>
-      <c r="K59" s="8" t="n">
+      <c r="K59" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5488,7 +5500,7 @@
       <c r="J60" s="0" t="n">
         <v>1.75</v>
       </c>
-      <c r="K60" s="8" t="n">
+      <c r="K60" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5523,7 +5535,7 @@
       <c r="J61" s="0" t="n">
         <v>1.44</v>
       </c>
-      <c r="K61" s="8" t="n">
+      <c r="K61" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5558,7 +5570,7 @@
       <c r="J62" s="0" t="n">
         <v>0.63</v>
       </c>
-      <c r="K62" s="8" t="n">
+      <c r="K62" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5593,7 +5605,7 @@
       <c r="J63" s="0" t="n">
         <v>2.15</v>
       </c>
-      <c r="K63" s="8" t="n">
+      <c r="K63" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5628,7 +5640,7 @@
       <c r="J64" s="0" t="n">
         <v>0.32</v>
       </c>
-      <c r="K64" s="8" t="n">
+      <c r="K64" s="7" t="n">
         <v>0.38</v>
       </c>
     </row>
@@ -5663,7 +5675,7 @@
       <c r="J65" s="0" t="n">
         <v>1.65</v>
       </c>
-      <c r="K65" s="8" t="n">
+      <c r="K65" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5698,7 +5710,7 @@
       <c r="J66" s="0" t="n">
         <v>0.46</v>
       </c>
-      <c r="K66" s="8" t="n">
+      <c r="K66" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5733,7 +5745,7 @@
       <c r="J67" s="0" t="n">
         <v>1.16</v>
       </c>
-      <c r="K67" s="8" t="n">
+      <c r="K67" s="7" t="n">
         <v>0.34</v>
       </c>
     </row>
@@ -5768,7 +5780,7 @@
       <c r="J68" s="0" t="n">
         <v>1.77</v>
       </c>
-      <c r="K68" s="8" t="n">
+      <c r="K68" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5803,7 +5815,7 @@
       <c r="J69" s="0" t="n">
         <v>1.91</v>
       </c>
-      <c r="K69" s="8" t="n">
+      <c r="K69" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5838,7 +5850,7 @@
       <c r="J70" s="0" t="n">
         <v>0.64</v>
       </c>
-      <c r="K70" s="8" t="n">
+      <c r="K70" s="7" t="n">
         <v>0.36</v>
       </c>
     </row>
@@ -5873,7 +5885,7 @@
       <c r="J71" s="0" t="n">
         <v>0.81</v>
       </c>
-      <c r="K71" s="8" t="n">
+      <c r="K71" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5898,8 +5910,8 @@
   </sheetPr>
   <dimension ref="A2:O24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A2:A74"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5907,10 +5919,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.53"/>
   </cols>
   <sheetData>
@@ -5921,7 +5933,7 @@
       <c r="C2" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="7" t="n">
+      <c r="D2" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5932,7 +5944,7 @@
       <c r="D3" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="E3" s="7" t="n">
+      <c r="E3" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5946,7 +5958,7 @@
       <c r="E4" s="0" t="n">
         <v>2.7</v>
       </c>
-      <c r="F4" s="7" t="n">
+      <c r="F4" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5963,7 +5975,7 @@
       <c r="F5" s="0" t="n">
         <v>5.15</v>
       </c>
-      <c r="G5" s="7" t="n">
+      <c r="G5" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5986,7 +5998,7 @@
       <c r="G6" s="0" t="n">
         <v>8.25</v>
       </c>
-      <c r="H6" s="7" t="n">
+      <c r="H6" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6009,7 +6021,7 @@
       <c r="H7" s="0" t="n">
         <v>4.33</v>
       </c>
-      <c r="I7" s="7" t="n">
+      <c r="I7" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6038,7 +6050,7 @@
       <c r="I8" s="0" t="n">
         <v>6.95</v>
       </c>
-      <c r="J8" s="7" t="n">
+      <c r="J8" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6070,7 +6082,7 @@
       <c r="J9" s="0" t="n">
         <v>2.5</v>
       </c>
-      <c r="K9" s="7" t="n">
+      <c r="K9" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6105,7 +6117,7 @@
       <c r="K10" s="0" t="n">
         <v>1.67</v>
       </c>
-      <c r="L10" s="7" t="n">
+      <c r="L10" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6143,7 +6155,7 @@
       <c r="L11" s="0" t="n">
         <v>11.85</v>
       </c>
-      <c r="M11" s="7" t="n">
+      <c r="M11" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6184,7 +6196,7 @@
       <c r="M12" s="0" t="n">
         <v>9.85</v>
       </c>
-      <c r="N12" s="7" t="n">
+      <c r="N12" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6228,7 +6240,7 @@
       <c r="N13" s="0" t="n">
         <v>7.5</v>
       </c>
-      <c r="O13" s="7" t="n">
+      <c r="O13" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6364,8 +6376,8 @@
   </sheetPr>
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="A2:A74 B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6851,13 +6863,14 @@
   </sheetPr>
   <dimension ref="A1:Q74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A74"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="4.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.43"/>
@@ -6867,7 +6880,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="8.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="9" width="8.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.53"/>
   </cols>
   <sheetData>
@@ -6875,8 +6888,8 @@
       <c r="A1" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
+      <c r="B1" s="0" t="s">
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -6905,7 +6918,7 @@
       <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="4" t="s">
         <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
@@ -6916,7 +6929,8 @@
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -6957,7 +6971,8 @@
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -6987,10 +7002,10 @@
       <c r="K3" s="0" t="n">
         <v>1.22</v>
       </c>
-      <c r="L3" s="6" t="n">
+      <c r="L3" s="9" t="n">
         <v>0.95</v>
       </c>
-      <c r="M3" s="0" t="s">
+      <c r="M3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6998,7 +7013,8 @@
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -7028,10 +7044,10 @@
       <c r="K4" s="0" t="n">
         <v>0.75</v>
       </c>
-      <c r="L4" s="0" t="n">
-        <v>95</v>
-      </c>
-      <c r="M4" s="0" t="s">
+      <c r="L4" s="9" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -7039,7 +7055,8 @@
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -7069,10 +7086,10 @@
       <c r="K5" s="0" t="n">
         <v>1.33</v>
       </c>
-      <c r="L5" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="M5" s="0" t="s">
+      <c r="L5" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -7080,7 +7097,8 @@
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -7110,59 +7128,61 @@
       <c r="K6" s="0" t="n">
         <v>0.6</v>
       </c>
-      <c r="L6" s="6" t="n">
+      <c r="L6" s="9" t="n">
         <v>0.9</v>
       </c>
-      <c r="M6" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="n">
+      <c r="B7" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="7" t="n">
+      <c r="D7" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="E7" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="7" t="s">
+      <c r="E7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="7" t="n">
+      <c r="H7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="I7" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="J7" s="7" t="s">
+      <c r="I7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J7" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="7" t="n">
+      <c r="K7" s="0" t="n">
         <v>0.79</v>
       </c>
-      <c r="L7" s="6" t="n">
+      <c r="L7" s="9" t="n">
         <v>0.9</v>
       </c>
-      <c r="M7" s="7" t="s">
-        <v>20</v>
+      <c r="M7" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -7192,10 +7212,10 @@
       <c r="K8" s="0" t="n">
         <v>0.08</v>
       </c>
-      <c r="L8" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="M8" s="0" t="s">
+      <c r="L8" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="M8" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -7203,7 +7223,8 @@
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -7233,7 +7254,7 @@
       <c r="K9" s="0" t="n">
         <v>0.95</v>
       </c>
-      <c r="L9" s="8" t="n">
+      <c r="L9" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M9" s="0" t="s">
@@ -7244,7 +7265,8 @@
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -7274,7 +7296,7 @@
       <c r="K10" s="0" t="n">
         <v>1.22</v>
       </c>
-      <c r="L10" s="8" t="n">
+      <c r="L10" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M10" s="0" t="s">
@@ -7285,7 +7307,8 @@
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -7315,7 +7338,7 @@
       <c r="K11" s="0" t="n">
         <v>0.71</v>
       </c>
-      <c r="L11" s="8" t="n">
+      <c r="L11" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M11" s="0" t="s">
@@ -7326,7 +7349,8 @@
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -7356,7 +7380,7 @@
       <c r="K12" s="0" t="n">
         <v>1.3</v>
       </c>
-      <c r="L12" s="8" t="n">
+      <c r="L12" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M12" s="0" t="s">
@@ -7367,7 +7391,8 @@
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -7397,7 +7422,7 @@
       <c r="K13" s="0" t="n">
         <v>0.47</v>
       </c>
-      <c r="L13" s="8" t="n">
+      <c r="L13" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M13" s="0" t="s">
@@ -7408,7 +7433,8 @@
       <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -7438,7 +7464,7 @@
       <c r="K14" s="0" t="n">
         <v>0.68</v>
       </c>
-      <c r="L14" s="8" t="n">
+      <c r="L14" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M14" s="0" t="s">
@@ -7449,7 +7475,8 @@
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -7479,7 +7506,7 @@
       <c r="K15" s="0" t="n">
         <v>1.28</v>
       </c>
-      <c r="L15" s="8" t="n">
+      <c r="L15" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M15" s="0" t="s">
@@ -7490,7 +7517,8 @@
       <c r="A16" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -7520,7 +7548,7 @@
       <c r="K16" s="0" t="n">
         <v>0.37</v>
       </c>
-      <c r="L16" s="8" t="n">
+      <c r="L16" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M16" s="0" t="s">
@@ -7531,7 +7559,8 @@
       <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -7561,7 +7590,7 @@
       <c r="K17" s="0" t="n">
         <v>0.89</v>
       </c>
-      <c r="L17" s="8" t="n">
+      <c r="L17" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M17" s="0" t="s">
@@ -7572,7 +7601,8 @@
       <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -7602,7 +7632,7 @@
       <c r="K18" s="0" t="n">
         <v>1.11</v>
       </c>
-      <c r="L18" s="8" t="n">
+      <c r="L18" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M18" s="0" t="s">
@@ -7613,7 +7643,8 @@
       <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -7643,7 +7674,7 @@
       <c r="K19" s="0" t="n">
         <v>0.9</v>
       </c>
-      <c r="L19" s="8" t="n">
+      <c r="L19" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M19" s="0" t="s">
@@ -7654,7 +7685,8 @@
       <c r="A20" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="0" t="n">
+      <c r="B20" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -7684,7 +7716,7 @@
       <c r="K20" s="0" t="n">
         <v>0.61</v>
       </c>
-      <c r="L20" s="8" t="n">
+      <c r="L20" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M20" s="0" t="s">
@@ -7695,7 +7727,8 @@
       <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="0" t="n">
+      <c r="B21" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -7725,7 +7758,7 @@
       <c r="K21" s="0" t="n">
         <v>0.16</v>
       </c>
-      <c r="L21" s="8" t="n">
+      <c r="L21" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M21" s="0" t="s">
@@ -7736,7 +7769,8 @@
       <c r="A22" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="0" t="n">
+      <c r="B22" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -7766,7 +7800,7 @@
       <c r="K22" s="0" t="n">
         <v>0.09</v>
       </c>
-      <c r="L22" s="8" t="n">
+      <c r="L22" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M22" s="0" t="s">
@@ -7777,7 +7811,8 @@
       <c r="A23" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="0" t="n">
+      <c r="B23" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -7807,10 +7842,10 @@
       <c r="K23" s="0" t="n">
         <v>5.78</v>
       </c>
-      <c r="L23" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M23" s="7" t="s">
+      <c r="L23" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -7818,7 +7853,8 @@
       <c r="A24" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="0" t="n">
+      <c r="B24" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -7848,10 +7884,10 @@
       <c r="K24" s="0" t="n">
         <v>5.36</v>
       </c>
-      <c r="L24" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M24" s="7" t="s">
+      <c r="L24" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -7859,7 +7895,8 @@
       <c r="A25" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="0" t="n">
+      <c r="B25" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -7889,10 +7926,10 @@
       <c r="K25" s="0" t="n">
         <v>2.85</v>
       </c>
-      <c r="L25" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M25" s="7" t="s">
+      <c r="L25" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -7900,7 +7937,8 @@
       <c r="A26" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="0" t="n">
+      <c r="B26" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C26" s="3" t="s">
@@ -7930,10 +7968,10 @@
       <c r="K26" s="0" t="n">
         <v>5.53</v>
       </c>
-      <c r="L26" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M26" s="7" t="s">
+      <c r="L26" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -7941,7 +7979,8 @@
       <c r="A27" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="0" t="n">
+      <c r="B27" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -7971,10 +8010,10 @@
       <c r="K27" s="0" t="n">
         <v>1.29</v>
       </c>
-      <c r="L27" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M27" s="7" t="s">
+      <c r="L27" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M27" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -7982,7 +8021,8 @@
       <c r="A28" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="0" t="n">
+      <c r="B28" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -8012,10 +8052,10 @@
       <c r="K28" s="0" t="n">
         <v>2.48</v>
       </c>
-      <c r="L28" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M28" s="7" t="s">
+      <c r="L28" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M28" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8023,7 +8063,8 @@
       <c r="A29" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="0" t="n">
+      <c r="B29" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -8053,10 +8094,10 @@
       <c r="K29" s="0" t="n">
         <v>5.65</v>
       </c>
-      <c r="L29" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M29" s="7" t="s">
+      <c r="L29" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M29" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8064,7 +8105,8 @@
       <c r="A30" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="0" t="n">
+      <c r="B30" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C30" s="3" t="s">
@@ -8094,10 +8136,10 @@
       <c r="K30" s="0" t="n">
         <v>2.8</v>
       </c>
-      <c r="L30" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M30" s="7" t="s">
+      <c r="L30" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8105,7 +8147,8 @@
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="0" t="n">
+      <c r="B31" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C31" s="3" t="s">
@@ -8135,10 +8178,10 @@
       <c r="K31" s="0" t="n">
         <v>4.32</v>
       </c>
-      <c r="L31" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M31" s="7" t="s">
+      <c r="L31" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M31" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8146,7 +8189,8 @@
       <c r="A32" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="0" t="n">
+      <c r="B32" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C32" s="3" t="s">
@@ -8176,10 +8220,10 @@
       <c r="K32" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="L32" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M32" s="7" t="s">
+      <c r="L32" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M32" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8187,7 +8231,8 @@
       <c r="A33" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="0" t="n">
+      <c r="B33" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -8217,10 +8262,10 @@
       <c r="K33" s="0" t="n">
         <v>2.53</v>
       </c>
-      <c r="L33" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M33" s="7" t="s">
+      <c r="L33" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8228,7 +8273,8 @@
       <c r="A34" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="0" t="n">
+      <c r="B34" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C34" s="3" t="s">
@@ -8258,10 +8304,10 @@
       <c r="K34" s="0" t="n">
         <v>4.48</v>
       </c>
-      <c r="L34" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M34" s="7" t="s">
+      <c r="L34" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M34" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8269,7 +8315,8 @@
       <c r="A35" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="0" t="n">
+      <c r="B35" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C35" s="3" t="s">
@@ -8299,10 +8346,10 @@
       <c r="K35" s="0" t="n">
         <v>8.15</v>
       </c>
-      <c r="L35" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M35" s="7" t="s">
+      <c r="L35" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M35" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8310,7 +8357,8 @@
       <c r="A36" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="B36" s="0" t="n">
+      <c r="B36" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C36" s="3" t="s">
@@ -8340,10 +8388,10 @@
       <c r="K36" s="0" t="n">
         <v>2.97</v>
       </c>
-      <c r="L36" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M36" s="7" t="s">
+      <c r="L36" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M36" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8351,7 +8399,8 @@
       <c r="A37" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="B37" s="0" t="n">
+      <c r="B37" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C37" s="3" t="s">
@@ -8381,10 +8430,10 @@
       <c r="K37" s="0" t="n">
         <v>4.3</v>
       </c>
-      <c r="L37" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M37" s="7" t="s">
+      <c r="L37" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M37" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8392,7 +8441,8 @@
       <c r="A38" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="B38" s="0" t="n">
+      <c r="B38" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -8422,7 +8472,7 @@
       <c r="K38" s="0" t="n">
         <v>0.41</v>
       </c>
-      <c r="L38" s="8" t="n">
+      <c r="L38" s="11" t="n">
         <v>0.53</v>
       </c>
       <c r="M38" s="0" t="s">
@@ -8433,7 +8483,8 @@
       <c r="A39" s="0" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="0" t="n">
+      <c r="B39" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -8463,7 +8514,7 @@
       <c r="K39" s="0" t="n">
         <v>0.16</v>
       </c>
-      <c r="L39" s="8" t="n">
+      <c r="L39" s="11" t="n">
         <v>0.66</v>
       </c>
       <c r="M39" s="0" t="s">
@@ -8474,7 +8525,8 @@
       <c r="A40" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="B40" s="0" t="n">
+      <c r="B40" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C40" s="3" t="s">
@@ -8504,7 +8556,7 @@
       <c r="K40" s="0" t="n">
         <v>1.22</v>
       </c>
-      <c r="L40" s="8" t="n">
+      <c r="L40" s="11" t="n">
         <v>0.51</v>
       </c>
       <c r="M40" s="0" t="s">
@@ -8515,7 +8567,8 @@
       <c r="A41" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="B41" s="0" t="n">
+      <c r="B41" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -8545,7 +8598,7 @@
       <c r="K41" s="0" t="n">
         <v>0.58</v>
       </c>
-      <c r="L41" s="8" t="n">
+      <c r="L41" s="11" t="n">
         <v>0.63</v>
       </c>
       <c r="M41" s="0" t="s">
@@ -8556,7 +8609,8 @@
       <c r="A42" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="B42" s="0" t="n">
+      <c r="B42" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C42" s="3" t="s">
@@ -8586,7 +8640,7 @@
       <c r="K42" s="0" t="n">
         <v>0.56</v>
       </c>
-      <c r="L42" s="8" t="n">
+      <c r="L42" s="11" t="n">
         <v>0.57</v>
       </c>
       <c r="M42" s="0" t="s">
@@ -8597,7 +8651,8 @@
       <c r="A43" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="B43" s="0" t="n">
+      <c r="B43" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -8627,7 +8682,7 @@
       <c r="K43" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="L43" s="8" t="n">
+      <c r="L43" s="11" t="n">
         <v>0.69</v>
       </c>
       <c r="M43" s="0" t="s">
@@ -8638,7 +8693,8 @@
       <c r="A44" s="0" t="n">
         <v>43</v>
       </c>
-      <c r="B44" s="0" t="n">
+      <c r="B44" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C44" s="2" t="s">
@@ -8668,7 +8724,7 @@
       <c r="K44" s="0" t="n">
         <v>1.18</v>
       </c>
-      <c r="L44" s="8" t="n">
+      <c r="L44" s="11" t="n">
         <v>0.71</v>
       </c>
       <c r="M44" s="0" t="s">
@@ -8679,7 +8735,8 @@
       <c r="A45" s="0" t="n">
         <v>44</v>
       </c>
-      <c r="B45" s="0" t="n">
+      <c r="B45" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C45" s="2" t="s">
@@ -8709,7 +8766,7 @@
       <c r="K45" s="0" t="n">
         <v>0.9</v>
       </c>
-      <c r="L45" s="8" t="n">
+      <c r="L45" s="11" t="n">
         <v>0.71</v>
       </c>
       <c r="M45" s="0" t="s">
@@ -8720,7 +8777,8 @@
       <c r="A46" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="B46" s="0" t="n">
+      <c r="B46" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C46" s="2" t="s">
@@ -8750,7 +8808,7 @@
       <c r="K46" s="0" t="n">
         <v>1.28</v>
       </c>
-      <c r="L46" s="8" t="n">
+      <c r="L46" s="11" t="n">
         <v>0.55</v>
       </c>
       <c r="M46" s="0" t="s">
@@ -8761,7 +8819,8 @@
       <c r="A47" s="0" t="n">
         <v>46</v>
       </c>
-      <c r="B47" s="0" t="n">
+      <c r="B47" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C47" s="2" t="s">
@@ -8791,7 +8850,7 @@
       <c r="K47" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="L47" s="8" t="n">
+      <c r="L47" s="11" t="n">
         <v>0.55</v>
       </c>
       <c r="M47" s="0" t="s">
@@ -8802,7 +8861,8 @@
       <c r="A48" s="0" t="n">
         <v>47</v>
       </c>
-      <c r="B48" s="0" t="n">
+      <c r="B48" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C48" s="2" t="s">
@@ -8832,7 +8892,7 @@
       <c r="K48" s="0" t="n">
         <v>0.95</v>
       </c>
-      <c r="L48" s="8" t="n">
+      <c r="L48" s="11" t="n">
         <v>0.69</v>
       </c>
       <c r="M48" s="0" t="s">
@@ -8843,7 +8903,8 @@
       <c r="A49" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="B49" s="0" t="n">
+      <c r="B49" s="10" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C49" s="2" t="s">
@@ -8873,7 +8934,7 @@
       <c r="K49" s="0" t="n">
         <v>0.95</v>
       </c>
-      <c r="L49" s="8" t="n">
+      <c r="L49" s="11" t="n">
         <v>0.69</v>
       </c>
       <c r="M49" s="0" t="s">
@@ -8884,7 +8945,8 @@
       <c r="A50" s="0" t="n">
         <v>49</v>
       </c>
-      <c r="B50" s="0" t="n">
+      <c r="B50" s="10" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C50" s="5" t="s">
@@ -8914,20 +8976,21 @@
       <c r="K50" s="0" t="n">
         <v>0.15</v>
       </c>
-      <c r="L50" s="8" t="n">
+      <c r="L50" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M50" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="P50" s="9"/>
-      <c r="Q50" s="8"/>
+        <v>40</v>
+      </c>
+      <c r="P50" s="8"/>
+      <c r="Q50" s="7"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="B51" s="0" t="n">
+      <c r="B51" s="10" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C51" s="3" t="s">
@@ -8957,19 +9020,20 @@
       <c r="K51" s="0" t="n">
         <v>1.68</v>
       </c>
-      <c r="L51" s="8" t="n">
+      <c r="L51" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M51" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q51" s="8"/>
+      <c r="Q51" s="7"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
         <v>51</v>
       </c>
-      <c r="B52" s="0" t="n">
+      <c r="B52" s="10" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C52" s="3" t="s">
@@ -8999,19 +9063,20 @@
       <c r="K52" s="0" t="n">
         <v>1.84</v>
       </c>
-      <c r="L52" s="8" t="n">
+      <c r="L52" s="11" t="n">
         <v>0.28</v>
       </c>
       <c r="M52" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q52" s="8"/>
+      <c r="Q52" s="7"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
         <v>52</v>
       </c>
-      <c r="B53" s="0" t="n">
+      <c r="B53" s="10" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C53" s="3" t="s">
@@ -9041,19 +9106,20 @@
       <c r="K53" s="0" t="n">
         <v>1.75</v>
       </c>
-      <c r="L53" s="8" t="n">
+      <c r="L53" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M53" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q53" s="8"/>
+      <c r="Q53" s="7"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
         <v>53</v>
       </c>
-      <c r="B54" s="0" t="n">
+      <c r="B54" s="10" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C54" s="3" t="s">
@@ -9083,19 +9149,20 @@
       <c r="K54" s="0" t="n">
         <v>0.77</v>
       </c>
-      <c r="L54" s="8" t="n">
+      <c r="L54" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M54" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q54" s="8"/>
+      <c r="Q54" s="7"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
         <v>54</v>
       </c>
-      <c r="B55" s="0" t="n">
+      <c r="B55" s="10" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C55" s="3" t="s">
@@ -9125,19 +9192,20 @@
       <c r="K55" s="0" t="n">
         <v>0.65</v>
       </c>
-      <c r="L55" s="8" t="n">
+      <c r="L55" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M55" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q55" s="8"/>
+      <c r="Q55" s="7"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="B56" s="0" t="n">
+      <c r="B56" s="10" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C56" s="3" t="s">
@@ -9167,19 +9235,20 @@
       <c r="K56" s="0" t="n">
         <v>0.68</v>
       </c>
-      <c r="L56" s="8" t="n">
+      <c r="L56" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M56" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q56" s="8"/>
+      <c r="Q56" s="7"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
         <v>56</v>
       </c>
-      <c r="B57" s="0" t="n">
+      <c r="B57" s="10" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C57" s="2" t="s">
@@ -9209,19 +9278,20 @@
       <c r="K57" s="0" t="n">
         <v>2.1</v>
       </c>
-      <c r="L57" s="8" t="n">
+      <c r="L57" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M57" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q57" s="8"/>
+      <c r="Q57" s="7"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
         <v>57</v>
       </c>
-      <c r="B58" s="0" t="n">
+      <c r="B58" s="10" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C58" s="2" t="s">
@@ -9251,19 +9321,20 @@
       <c r="K58" s="0" t="n">
         <v>1.76</v>
       </c>
-      <c r="L58" s="8" t="n">
+      <c r="L58" s="11" t="n">
         <v>0.26</v>
       </c>
       <c r="M58" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q58" s="8"/>
+      <c r="Q58" s="7"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
         <v>58</v>
       </c>
-      <c r="B59" s="0" t="n">
+      <c r="B59" s="10" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C59" s="2" t="s">
@@ -9293,19 +9364,20 @@
       <c r="K59" s="0" t="n">
         <v>0.05</v>
       </c>
-      <c r="L59" s="8" t="n">
+      <c r="L59" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M59" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q59" s="8"/>
+      <c r="Q59" s="7"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="B60" s="0" t="n">
+      <c r="B60" s="10" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C60" s="2" t="s">
@@ -9335,19 +9407,20 @@
       <c r="K60" s="0" t="n">
         <v>2.43</v>
       </c>
-      <c r="L60" s="8" t="n">
+      <c r="L60" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M60" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q60" s="8"/>
+      <c r="Q60" s="7"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="B61" s="0" t="n">
+      <c r="B61" s="10" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C61" s="5" t="s">
@@ -9377,19 +9450,20 @@
       <c r="K61" s="0" t="n">
         <v>0.34</v>
       </c>
-      <c r="L61" s="8" t="n">
+      <c r="L61" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M61" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q61" s="8"/>
+      <c r="Q61" s="7"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
         <v>61</v>
       </c>
-      <c r="B62" s="0" t="n">
+      <c r="B62" s="10" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C62" s="2" t="s">
@@ -9419,19 +9493,20 @@
       <c r="K62" s="0" t="n">
         <v>1.75</v>
       </c>
-      <c r="L62" s="8" t="n">
+      <c r="L62" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M62" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q62" s="8"/>
+      <c r="Q62" s="7"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
         <v>62</v>
       </c>
-      <c r="B63" s="0" t="n">
+      <c r="B63" s="10" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C63" s="5" t="s">
@@ -9461,19 +9536,20 @@
       <c r="K63" s="0" t="n">
         <v>1.75</v>
       </c>
-      <c r="L63" s="8" t="n">
+      <c r="L63" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M63" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q63" s="8"/>
+      <c r="Q63" s="7"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
         <v>63</v>
       </c>
-      <c r="B64" s="0" t="n">
+      <c r="B64" s="10" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C64" s="3" t="s">
@@ -9503,19 +9579,20 @@
       <c r="K64" s="0" t="n">
         <v>1.44</v>
       </c>
-      <c r="L64" s="8" t="n">
+      <c r="L64" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M64" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q64" s="8"/>
+      <c r="Q64" s="7"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
         <v>64</v>
       </c>
-      <c r="B65" s="0" t="n">
+      <c r="B65" s="10" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C65" s="3" t="s">
@@ -9545,19 +9622,20 @@
       <c r="K65" s="0" t="n">
         <v>0.63</v>
       </c>
-      <c r="L65" s="8" t="n">
+      <c r="L65" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M65" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q65" s="8"/>
+      <c r="Q65" s="7"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="B66" s="0" t="n">
+      <c r="B66" s="10" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C66" s="3" t="s">
@@ -9587,19 +9665,20 @@
       <c r="K66" s="0" t="n">
         <v>2.15</v>
       </c>
-      <c r="L66" s="8" t="n">
+      <c r="L66" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M66" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q66" s="8"/>
+      <c r="Q66" s="7"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
         <v>66</v>
       </c>
-      <c r="B67" s="0" t="n">
+      <c r="B67" s="10" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C67" s="2" t="s">
@@ -9629,19 +9708,20 @@
       <c r="K67" s="0" t="n">
         <v>0.32</v>
       </c>
-      <c r="L67" s="8" t="n">
+      <c r="L67" s="11" t="n">
         <v>0.38</v>
       </c>
       <c r="M67" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="Q67" s="8"/>
+      <c r="Q67" s="7"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
         <v>67</v>
       </c>
-      <c r="B68" s="0" t="n">
+      <c r="B68" s="10" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C68" s="2" t="s">
@@ -9671,20 +9751,21 @@
       <c r="K68" s="0" t="n">
         <v>1.65</v>
       </c>
-      <c r="L68" s="8" t="n">
+      <c r="L68" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M68" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="P68" s="9"/>
-      <c r="Q68" s="8"/>
+      <c r="P68" s="8"/>
+      <c r="Q68" s="7"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
         <v>68</v>
       </c>
-      <c r="B69" s="0" t="n">
+      <c r="B69" s="10" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C69" s="2" t="s">
@@ -9714,20 +9795,21 @@
       <c r="K69" s="0" t="n">
         <v>0.46</v>
       </c>
-      <c r="L69" s="8" t="n">
+      <c r="L69" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M69" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="P69" s="9"/>
-      <c r="Q69" s="8"/>
+      <c r="P69" s="8"/>
+      <c r="Q69" s="7"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
         <v>69</v>
       </c>
-      <c r="B70" s="0" t="n">
+      <c r="B70" s="10" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C70" s="2" t="s">
@@ -9757,20 +9839,21 @@
       <c r="K70" s="0" t="n">
         <v>1.16</v>
       </c>
-      <c r="L70" s="8" t="n">
+      <c r="L70" s="11" t="n">
         <v>0.34</v>
       </c>
       <c r="M70" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="P70" s="9"/>
-      <c r="Q70" s="8"/>
+      <c r="P70" s="8"/>
+      <c r="Q70" s="7"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
         <v>70</v>
       </c>
-      <c r="B71" s="0" t="n">
+      <c r="B71" s="10" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C71" s="2" t="s">
@@ -9800,20 +9883,21 @@
       <c r="K71" s="0" t="n">
         <v>1.77</v>
       </c>
-      <c r="L71" s="8" t="n">
+      <c r="L71" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M71" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P71" s="9"/>
-      <c r="Q71" s="8"/>
+      <c r="P71" s="8"/>
+      <c r="Q71" s="7"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="B72" s="0" t="n">
+      <c r="B72" s="10" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C72" s="2" t="s">
@@ -9843,20 +9927,21 @@
       <c r="K72" s="0" t="n">
         <v>1.91</v>
       </c>
-      <c r="L72" s="8" t="n">
+      <c r="L72" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M72" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P72" s="9"/>
-      <c r="Q72" s="8"/>
+      <c r="P72" s="8"/>
+      <c r="Q72" s="7"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
         <v>72</v>
       </c>
-      <c r="B73" s="0" t="n">
+      <c r="B73" s="10" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C73" s="3" t="s">
@@ -9886,20 +9971,21 @@
       <c r="K73" s="0" t="n">
         <v>0.64</v>
       </c>
-      <c r="L73" s="8" t="n">
+      <c r="L73" s="11" t="n">
         <v>0.36</v>
       </c>
       <c r="M73" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P73" s="9"/>
-      <c r="Q73" s="8"/>
+      <c r="P73" s="8"/>
+      <c r="Q73" s="7"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
         <v>73</v>
       </c>
-      <c r="B74" s="0" t="n">
+      <c r="B74" s="10" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C74" s="3" t="s">
@@ -9929,14 +10015,14 @@
       <c r="K74" s="0" t="n">
         <v>0.81</v>
       </c>
-      <c r="L74" s="8" t="n">
+      <c r="L74" s="11" t="n">
         <v>0</v>
       </c>
       <c r="M74" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="P74" s="9"/>
-      <c r="Q74" s="8"/>
+      <c r="P74" s="8"/>
+      <c r="Q74" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Added TODOs for analysis ideas
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -211,12 +211,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00%"/>
     <numFmt numFmtId="166" formatCode="0%"/>
     <numFmt numFmtId="167" formatCode="0"/>
-    <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="168" formatCode="0.00"/>
+    <numFmt numFmtId="169" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -248,7 +249,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -271,6 +272,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FF993300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF58220"/>
+        <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
   </fills>
@@ -310,7 +317,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -339,6 +346,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -347,11 +358,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -414,7 +433,7 @@
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFF58220"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
@@ -438,8 +457,8 @@
   </sheetPr>
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A50" activeCellId="0" sqref="A50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -763,7 +782,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="7" t="n">
         <v>0</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -793,7 +812,7 @@
       <c r="J9" s="0" t="n">
         <v>0.95</v>
       </c>
-      <c r="K9" s="7" t="n">
+      <c r="K9" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L9" s="0" t="s">
@@ -831,7 +850,7 @@
       <c r="J10" s="0" t="n">
         <v>1.22</v>
       </c>
-      <c r="K10" s="7" t="n">
+      <c r="K10" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L10" s="0" t="s">
@@ -839,7 +858,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="7" t="n">
         <v>0</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -869,7 +888,7 @@
       <c r="J11" s="0" t="n">
         <v>0.71</v>
       </c>
-      <c r="K11" s="7" t="n">
+      <c r="K11" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L11" s="0" t="s">
@@ -907,7 +926,7 @@
       <c r="J12" s="0" t="n">
         <v>1.3</v>
       </c>
-      <c r="K12" s="7" t="n">
+      <c r="K12" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L12" s="0" t="s">
@@ -915,7 +934,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="7" t="n">
         <v>0</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -945,7 +964,7 @@
       <c r="J13" s="0" t="n">
         <v>0.47</v>
       </c>
-      <c r="K13" s="7" t="n">
+      <c r="K13" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L13" s="0" t="s">
@@ -953,7 +972,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="7" t="n">
         <v>0</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -983,7 +1002,7 @@
       <c r="J14" s="0" t="n">
         <v>0.68</v>
       </c>
-      <c r="K14" s="7" t="n">
+      <c r="K14" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L14" s="0" t="s">
@@ -1021,7 +1040,7 @@
       <c r="J15" s="0" t="n">
         <v>1.28</v>
       </c>
-      <c r="K15" s="7" t="n">
+      <c r="K15" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L15" s="0" t="s">
@@ -1059,7 +1078,7 @@
       <c r="J16" s="0" t="n">
         <v>0.37</v>
       </c>
-      <c r="K16" s="7" t="n">
+      <c r="K16" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L16" s="0" t="s">
@@ -1097,7 +1116,7 @@
       <c r="J17" s="0" t="n">
         <v>0.89</v>
       </c>
-      <c r="K17" s="7" t="n">
+      <c r="K17" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L17" s="0" t="s">
@@ -1135,7 +1154,7 @@
       <c r="J18" s="0" t="n">
         <v>1.11</v>
       </c>
-      <c r="K18" s="7" t="n">
+      <c r="K18" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L18" s="0" t="s">
@@ -1173,7 +1192,7 @@
       <c r="J19" s="0" t="n">
         <v>0.9</v>
       </c>
-      <c r="K19" s="7" t="n">
+      <c r="K19" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L19" s="0" t="s">
@@ -1211,7 +1230,7 @@
       <c r="J20" s="0" t="n">
         <v>0.61</v>
       </c>
-      <c r="K20" s="7" t="n">
+      <c r="K20" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L20" s="0" t="s">
@@ -1249,7 +1268,7 @@
       <c r="J21" s="0" t="n">
         <v>0.16</v>
       </c>
-      <c r="K21" s="7" t="n">
+      <c r="K21" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L21" s="0" t="s">
@@ -1287,7 +1306,7 @@
       <c r="J22" s="0" t="n">
         <v>0.09</v>
       </c>
-      <c r="K22" s="7" t="n">
+      <c r="K22" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L22" s="0" t="s">
@@ -1325,7 +1344,7 @@
       <c r="J23" s="0" t="n">
         <v>5.78</v>
       </c>
-      <c r="K23" s="7" t="n">
+      <c r="K23" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L23" s="0" t="s">
@@ -1363,7 +1382,7 @@
       <c r="J24" s="0" t="n">
         <v>5.36</v>
       </c>
-      <c r="K24" s="7" t="n">
+      <c r="K24" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L24" s="0" t="s">
@@ -1401,7 +1420,7 @@
       <c r="J25" s="0" t="n">
         <v>2.85</v>
       </c>
-      <c r="K25" s="7" t="n">
+      <c r="K25" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L25" s="0" t="s">
@@ -1439,7 +1458,7 @@
       <c r="J26" s="0" t="n">
         <v>5.53</v>
       </c>
-      <c r="K26" s="7" t="n">
+      <c r="K26" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L26" s="0" t="s">
@@ -1477,7 +1496,7 @@
       <c r="J27" s="0" t="n">
         <v>1.29</v>
       </c>
-      <c r="K27" s="7" t="n">
+      <c r="K27" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L27" s="0" t="s">
@@ -1515,7 +1534,7 @@
       <c r="J28" s="0" t="n">
         <v>2.48</v>
       </c>
-      <c r="K28" s="7" t="n">
+      <c r="K28" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L28" s="0" t="s">
@@ -1553,7 +1572,7 @@
       <c r="J29" s="0" t="n">
         <v>5.65</v>
       </c>
-      <c r="K29" s="7" t="n">
+      <c r="K29" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L29" s="0" t="s">
@@ -1591,7 +1610,7 @@
       <c r="J30" s="0" t="n">
         <v>2.8</v>
       </c>
-      <c r="K30" s="7" t="n">
+      <c r="K30" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L30" s="0" t="s">
@@ -1629,7 +1648,7 @@
       <c r="J31" s="0" t="n">
         <v>4.32</v>
       </c>
-      <c r="K31" s="7" t="n">
+      <c r="K31" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L31" s="0" t="s">
@@ -1667,7 +1686,7 @@
       <c r="J32" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="K32" s="7" t="n">
+      <c r="K32" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L32" s="0" t="s">
@@ -1705,7 +1724,7 @@
       <c r="J33" s="0" t="n">
         <v>2.53</v>
       </c>
-      <c r="K33" s="7" t="n">
+      <c r="K33" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L33" s="0" t="s">
@@ -1743,7 +1762,7 @@
       <c r="J34" s="0" t="n">
         <v>4.48</v>
       </c>
-      <c r="K34" s="7" t="n">
+      <c r="K34" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L34" s="0" t="s">
@@ -1781,7 +1800,7 @@
       <c r="J35" s="0" t="n">
         <v>8.15</v>
       </c>
-      <c r="K35" s="7" t="n">
+      <c r="K35" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L35" s="0" t="s">
@@ -1819,7 +1838,7 @@
       <c r="J36" s="0" t="n">
         <v>2.97</v>
       </c>
-      <c r="K36" s="7" t="n">
+      <c r="K36" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L36" s="0" t="s">
@@ -1857,7 +1876,7 @@
       <c r="J37" s="0" t="n">
         <v>4.3</v>
       </c>
-      <c r="K37" s="7" t="n">
+      <c r="K37" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L37" s="0" t="s">
@@ -1895,7 +1914,7 @@
       <c r="J38" s="0" t="n">
         <v>0.41</v>
       </c>
-      <c r="K38" s="7" t="n">
+      <c r="K38" s="8" t="n">
         <v>0.53</v>
       </c>
       <c r="L38" s="0" t="s">
@@ -1933,7 +1952,7 @@
       <c r="J39" s="0" t="n">
         <v>0.16</v>
       </c>
-      <c r="K39" s="7" t="n">
+      <c r="K39" s="8" t="n">
         <v>0.66</v>
       </c>
       <c r="L39" s="0" t="s">
@@ -1971,7 +1990,7 @@
       <c r="J40" s="0" t="n">
         <v>1.22</v>
       </c>
-      <c r="K40" s="7" t="n">
+      <c r="K40" s="8" t="n">
         <v>0.51</v>
       </c>
       <c r="L40" s="0" t="s">
@@ -2009,7 +2028,7 @@
       <c r="J41" s="0" t="n">
         <v>0.58</v>
       </c>
-      <c r="K41" s="7" t="n">
+      <c r="K41" s="8" t="n">
         <v>0.63</v>
       </c>
       <c r="L41" s="0" t="s">
@@ -2047,7 +2066,7 @@
       <c r="J42" s="0" t="n">
         <v>0.56</v>
       </c>
-      <c r="K42" s="7" t="n">
+      <c r="K42" s="8" t="n">
         <v>0.57</v>
       </c>
       <c r="L42" s="0" t="s">
@@ -2085,7 +2104,7 @@
       <c r="J43" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="K43" s="7" t="n">
+      <c r="K43" s="8" t="n">
         <v>0.69</v>
       </c>
       <c r="L43" s="0" t="s">
@@ -2123,7 +2142,7 @@
       <c r="J44" s="0" t="n">
         <v>1.18</v>
       </c>
-      <c r="K44" s="7" t="n">
+      <c r="K44" s="8" t="n">
         <v>0.71</v>
       </c>
       <c r="L44" s="0" t="s">
@@ -2161,7 +2180,7 @@
       <c r="J45" s="0" t="n">
         <v>0.9</v>
       </c>
-      <c r="K45" s="7" t="n">
+      <c r="K45" s="8" t="n">
         <v>0.71</v>
       </c>
       <c r="L45" s="0" t="s">
@@ -2199,7 +2218,7 @@
       <c r="J46" s="0" t="n">
         <v>1.28</v>
       </c>
-      <c r="K46" s="7" t="n">
+      <c r="K46" s="8" t="n">
         <v>0.55</v>
       </c>
       <c r="L46" s="0" t="s">
@@ -2237,7 +2256,7 @@
       <c r="J47" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K47" s="7" t="n">
+      <c r="K47" s="8" t="n">
         <v>0.55</v>
       </c>
       <c r="L47" s="0" t="s">
@@ -2275,7 +2294,7 @@
       <c r="J48" s="0" t="n">
         <v>0.95</v>
       </c>
-      <c r="K48" s="7" t="n">
+      <c r="K48" s="8" t="n">
         <v>0.69</v>
       </c>
       <c r="L48" s="0" t="s">
@@ -2313,7 +2332,7 @@
       <c r="J49" s="0" t="n">
         <v>0.95</v>
       </c>
-      <c r="K49" s="7" t="n">
+      <c r="K49" s="8" t="n">
         <v>0.69</v>
       </c>
       <c r="L49" s="0" t="s">
@@ -2443,14 +2462,14 @@
       <c r="J2" s="0" t="n">
         <v>0.15</v>
       </c>
-      <c r="K2" s="7" t="n">
+      <c r="K2" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L2" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="8"/>
-      <c r="P2" s="7"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -2483,13 +2502,13 @@
       <c r="J3" s="0" t="n">
         <v>1.68</v>
       </c>
-      <c r="K3" s="7" t="n">
+      <c r="K3" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L3" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P3" s="7"/>
+      <c r="P3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -2522,13 +2541,13 @@
       <c r="J4" s="0" t="n">
         <v>1.84</v>
       </c>
-      <c r="K4" s="7" t="n">
+      <c r="K4" s="8" t="n">
         <v>0.28</v>
       </c>
       <c r="L4" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P4" s="7"/>
+      <c r="P4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -2561,13 +2580,13 @@
       <c r="J5" s="0" t="n">
         <v>1.75</v>
       </c>
-      <c r="K5" s="7" t="n">
+      <c r="K5" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L5" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P5" s="7"/>
+      <c r="P5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -2600,13 +2619,13 @@
       <c r="J6" s="0" t="n">
         <v>0.77</v>
       </c>
-      <c r="K6" s="7" t="n">
+      <c r="K6" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L6" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P6" s="7"/>
+      <c r="P6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -2639,13 +2658,13 @@
       <c r="J7" s="0" t="n">
         <v>0.65</v>
       </c>
-      <c r="K7" s="7" t="n">
+      <c r="K7" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L7" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P7" s="7"/>
+      <c r="P7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -2678,13 +2697,13 @@
       <c r="J8" s="0" t="n">
         <v>0.68</v>
       </c>
-      <c r="K8" s="7" t="n">
+      <c r="K8" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L8" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P8" s="7"/>
+      <c r="P8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -2717,13 +2736,13 @@
       <c r="J9" s="0" t="n">
         <v>2.1</v>
       </c>
-      <c r="K9" s="7" t="n">
+      <c r="K9" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L9" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P9" s="7"/>
+      <c r="P9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -2756,13 +2775,13 @@
       <c r="J10" s="0" t="n">
         <v>1.76</v>
       </c>
-      <c r="K10" s="7" t="n">
+      <c r="K10" s="8" t="n">
         <v>0.26</v>
       </c>
       <c r="L10" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P10" s="7"/>
+      <c r="P10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -2795,13 +2814,13 @@
       <c r="J11" s="0" t="n">
         <v>0.05</v>
       </c>
-      <c r="K11" s="7" t="n">
+      <c r="K11" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L11" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P11" s="7"/>
+      <c r="P11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -2834,13 +2853,13 @@
       <c r="J12" s="0" t="n">
         <v>2.43</v>
       </c>
-      <c r="K12" s="7" t="n">
+      <c r="K12" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L12" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P12" s="7"/>
+      <c r="P12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -2873,13 +2892,13 @@
       <c r="J13" s="0" t="n">
         <v>0.34</v>
       </c>
-      <c r="K13" s="7" t="n">
+      <c r="K13" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L13" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P13" s="7"/>
+      <c r="P13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -2912,13 +2931,13 @@
       <c r="J14" s="0" t="n">
         <v>1.75</v>
       </c>
-      <c r="K14" s="7" t="n">
+      <c r="K14" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L14" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P14" s="7"/>
+      <c r="P14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -2951,13 +2970,13 @@
       <c r="J15" s="0" t="n">
         <v>1.75</v>
       </c>
-      <c r="K15" s="7" t="n">
+      <c r="K15" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L15" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P15" s="7"/>
+      <c r="P15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -2990,13 +3009,13 @@
       <c r="J16" s="0" t="n">
         <v>1.44</v>
       </c>
-      <c r="K16" s="7" t="n">
+      <c r="K16" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L16" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P16" s="7"/>
+      <c r="P16" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
@@ -3029,13 +3048,13 @@
       <c r="J17" s="0" t="n">
         <v>0.63</v>
       </c>
-      <c r="K17" s="7" t="n">
+      <c r="K17" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L17" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P17" s="7"/>
+      <c r="P17" s="8"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
@@ -3068,13 +3087,13 @@
       <c r="J18" s="0" t="n">
         <v>2.15</v>
       </c>
-      <c r="K18" s="7" t="n">
+      <c r="K18" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L18" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P18" s="7"/>
+      <c r="P18" s="8"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
@@ -3107,13 +3126,13 @@
       <c r="J19" s="0" t="n">
         <v>0.32</v>
       </c>
-      <c r="K19" s="7" t="n">
+      <c r="K19" s="8" t="n">
         <v>0.38</v>
       </c>
       <c r="L19" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="P19" s="7"/>
+      <c r="P19" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -3146,14 +3165,14 @@
       <c r="J20" s="0" t="n">
         <v>1.65</v>
       </c>
-      <c r="K20" s="7" t="n">
+      <c r="K20" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L20" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="O20" s="8"/>
-      <c r="P20" s="7"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="8"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
@@ -3186,14 +3205,14 @@
       <c r="J21" s="0" t="n">
         <v>0.46</v>
       </c>
-      <c r="K21" s="7" t="n">
+      <c r="K21" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L21" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="O21" s="8"/>
-      <c r="P21" s="7"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="8"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
@@ -3226,14 +3245,14 @@
       <c r="J22" s="0" t="n">
         <v>1.16</v>
       </c>
-      <c r="K22" s="7" t="n">
+      <c r="K22" s="8" t="n">
         <v>0.34</v>
       </c>
       <c r="L22" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="O22" s="8"/>
-      <c r="P22" s="7"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="8"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -3266,14 +3285,14 @@
       <c r="J23" s="0" t="n">
         <v>1.77</v>
       </c>
-      <c r="K23" s="7" t="n">
+      <c r="K23" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L23" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="O23" s="8"/>
-      <c r="P23" s="7"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="8"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
@@ -3306,14 +3325,14 @@
       <c r="J24" s="0" t="n">
         <v>1.91</v>
       </c>
-      <c r="K24" s="7" t="n">
+      <c r="K24" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L24" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="O24" s="8"/>
-      <c r="P24" s="7"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="8"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
@@ -3346,14 +3365,14 @@
       <c r="J25" s="0" t="n">
         <v>0.64</v>
       </c>
-      <c r="K25" s="7" t="n">
+      <c r="K25" s="8" t="n">
         <v>0.36</v>
       </c>
       <c r="L25" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="O25" s="8"/>
-      <c r="P25" s="7"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="8"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
@@ -3386,14 +3405,14 @@
       <c r="J26" s="0" t="n">
         <v>0.81</v>
       </c>
-      <c r="K26" s="7" t="n">
+      <c r="K26" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L26" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="O26" s="8"/>
-      <c r="P26" s="7"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3470,7 +3489,7 @@
       <c r="J2" s="0" t="n">
         <v>0.15</v>
       </c>
-      <c r="K2" s="7" t="n">
+      <c r="K2" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3715,7 +3734,7 @@
       <c r="J9" s="0" t="n">
         <v>0.95</v>
       </c>
-      <c r="K9" s="7" t="n">
+      <c r="K9" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3750,7 +3769,7 @@
       <c r="J10" s="0" t="n">
         <v>1.22</v>
       </c>
-      <c r="K10" s="7" t="n">
+      <c r="K10" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3785,7 +3804,7 @@
       <c r="J11" s="0" t="n">
         <v>0.71</v>
       </c>
-      <c r="K11" s="7" t="n">
+      <c r="K11" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3820,7 +3839,7 @@
       <c r="J12" s="0" t="n">
         <v>1.3</v>
       </c>
-      <c r="K12" s="7" t="n">
+      <c r="K12" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3855,7 +3874,7 @@
       <c r="J13" s="0" t="n">
         <v>0.47</v>
       </c>
-      <c r="K13" s="7" t="n">
+      <c r="K13" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3890,7 +3909,7 @@
       <c r="J14" s="0" t="n">
         <v>0.68</v>
       </c>
-      <c r="K14" s="7" t="n">
+      <c r="K14" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3925,7 +3944,7 @@
       <c r="J15" s="0" t="n">
         <v>1.28</v>
       </c>
-      <c r="K15" s="7" t="n">
+      <c r="K15" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3960,7 +3979,7 @@
       <c r="J16" s="0" t="n">
         <v>0.37</v>
       </c>
-      <c r="K16" s="7" t="n">
+      <c r="K16" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3995,7 +4014,7 @@
       <c r="J17" s="0" t="n">
         <v>0.89</v>
       </c>
-      <c r="K17" s="7" t="n">
+      <c r="K17" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4030,7 +4049,7 @@
       <c r="J18" s="0" t="n">
         <v>1.11</v>
       </c>
-      <c r="K18" s="7" t="n">
+      <c r="K18" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4065,7 +4084,7 @@
       <c r="J19" s="0" t="n">
         <v>0.9</v>
       </c>
-      <c r="K19" s="7" t="n">
+      <c r="K19" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4100,7 +4119,7 @@
       <c r="J20" s="0" t="n">
         <v>0.61</v>
       </c>
-      <c r="K20" s="7" t="n">
+      <c r="K20" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4135,7 +4154,7 @@
       <c r="J21" s="0" t="n">
         <v>0.16</v>
       </c>
-      <c r="K21" s="7" t="n">
+      <c r="K21" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4170,7 +4189,7 @@
       <c r="J22" s="0" t="n">
         <v>0.09</v>
       </c>
-      <c r="K22" s="7" t="n">
+      <c r="K22" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4205,7 +4224,7 @@
       <c r="J23" s="0" t="n">
         <v>5.78</v>
       </c>
-      <c r="K23" s="7" t="n">
+      <c r="K23" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4240,7 +4259,7 @@
       <c r="J24" s="0" t="n">
         <v>5.36</v>
       </c>
-      <c r="K24" s="7" t="n">
+      <c r="K24" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4275,7 +4294,7 @@
       <c r="J25" s="0" t="n">
         <v>2.85</v>
       </c>
-      <c r="K25" s="7" t="n">
+      <c r="K25" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4310,7 +4329,7 @@
       <c r="J26" s="0" t="n">
         <v>5.53</v>
       </c>
-      <c r="K26" s="7" t="n">
+      <c r="K26" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4345,7 +4364,7 @@
       <c r="J27" s="0" t="n">
         <v>1.29</v>
       </c>
-      <c r="K27" s="7" t="n">
+      <c r="K27" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4380,7 +4399,7 @@
       <c r="J28" s="0" t="n">
         <v>2.48</v>
       </c>
-      <c r="K28" s="7" t="n">
+      <c r="K28" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4415,7 +4434,7 @@
       <c r="J29" s="0" t="n">
         <v>5.65</v>
       </c>
-      <c r="K29" s="7" t="n">
+      <c r="K29" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4450,7 +4469,7 @@
       <c r="J30" s="0" t="n">
         <v>2.8</v>
       </c>
-      <c r="K30" s="7" t="n">
+      <c r="K30" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4485,7 +4504,7 @@
       <c r="J31" s="0" t="n">
         <v>4.32</v>
       </c>
-      <c r="K31" s="7" t="n">
+      <c r="K31" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4520,7 +4539,7 @@
       <c r="J32" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="K32" s="7" t="n">
+      <c r="K32" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4555,7 +4574,7 @@
       <c r="J33" s="0" t="n">
         <v>2.53</v>
       </c>
-      <c r="K33" s="7" t="n">
+      <c r="K33" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4590,7 +4609,7 @@
       <c r="J34" s="0" t="n">
         <v>4.48</v>
       </c>
-      <c r="K34" s="7" t="n">
+      <c r="K34" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4625,7 +4644,7 @@
       <c r="J35" s="0" t="n">
         <v>8.15</v>
       </c>
-      <c r="K35" s="7" t="n">
+      <c r="K35" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4660,7 +4679,7 @@
       <c r="J36" s="0" t="n">
         <v>2.97</v>
       </c>
-      <c r="K36" s="7" t="n">
+      <c r="K36" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4695,7 +4714,7 @@
       <c r="J37" s="0" t="n">
         <v>4.3</v>
       </c>
-      <c r="K37" s="7" t="n">
+      <c r="K37" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4730,7 +4749,7 @@
       <c r="J38" s="0" t="n">
         <v>0.41</v>
       </c>
-      <c r="K38" s="7" t="n">
+      <c r="K38" s="8" t="n">
         <v>0.53</v>
       </c>
     </row>
@@ -4765,7 +4784,7 @@
       <c r="J39" s="0" t="n">
         <v>0.16</v>
       </c>
-      <c r="K39" s="7" t="n">
+      <c r="K39" s="8" t="n">
         <v>0.66</v>
       </c>
     </row>
@@ -4800,7 +4819,7 @@
       <c r="J40" s="0" t="n">
         <v>1.22</v>
       </c>
-      <c r="K40" s="7" t="n">
+      <c r="K40" s="8" t="n">
         <v>0.51</v>
       </c>
     </row>
@@ -4835,7 +4854,7 @@
       <c r="J41" s="0" t="n">
         <v>0.58</v>
       </c>
-      <c r="K41" s="7" t="n">
+      <c r="K41" s="8" t="n">
         <v>0.63</v>
       </c>
     </row>
@@ -4870,7 +4889,7 @@
       <c r="J42" s="0" t="n">
         <v>0.56</v>
       </c>
-      <c r="K42" s="7" t="n">
+      <c r="K42" s="8" t="n">
         <v>0.57</v>
       </c>
     </row>
@@ -4905,7 +4924,7 @@
       <c r="J43" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="K43" s="7" t="n">
+      <c r="K43" s="8" t="n">
         <v>0.69</v>
       </c>
     </row>
@@ -4940,7 +4959,7 @@
       <c r="J44" s="0" t="n">
         <v>1.18</v>
       </c>
-      <c r="K44" s="7" t="n">
+      <c r="K44" s="8" t="n">
         <v>0.71</v>
       </c>
     </row>
@@ -4975,7 +4994,7 @@
       <c r="J45" s="0" t="n">
         <v>0.9</v>
       </c>
-      <c r="K45" s="7" t="n">
+      <c r="K45" s="8" t="n">
         <v>0.71</v>
       </c>
     </row>
@@ -5010,7 +5029,7 @@
       <c r="J46" s="0" t="n">
         <v>1.28</v>
       </c>
-      <c r="K46" s="7" t="n">
+      <c r="K46" s="8" t="n">
         <v>0.55</v>
       </c>
     </row>
@@ -5045,7 +5064,7 @@
       <c r="J47" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K47" s="7" t="n">
+      <c r="K47" s="8" t="n">
         <v>0.55</v>
       </c>
     </row>
@@ -5080,7 +5099,7 @@
       <c r="J48" s="0" t="n">
         <v>0.95</v>
       </c>
-      <c r="K48" s="7" t="n">
+      <c r="K48" s="8" t="n">
         <v>0.69</v>
       </c>
     </row>
@@ -5115,7 +5134,7 @@
       <c r="J49" s="0" t="n">
         <v>1.68</v>
       </c>
-      <c r="K49" s="7" t="n">
+      <c r="K49" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5150,7 +5169,7 @@
       <c r="J50" s="0" t="n">
         <v>1.84</v>
       </c>
-      <c r="K50" s="7" t="n">
+      <c r="K50" s="8" t="n">
         <v>0.28</v>
       </c>
     </row>
@@ -5185,7 +5204,7 @@
       <c r="J51" s="0" t="n">
         <v>1.75</v>
       </c>
-      <c r="K51" s="7" t="n">
+      <c r="K51" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5220,7 +5239,7 @@
       <c r="J52" s="0" t="n">
         <v>0.77</v>
       </c>
-      <c r="K52" s="7" t="n">
+      <c r="K52" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5255,7 +5274,7 @@
       <c r="J53" s="0" t="n">
         <v>0.65</v>
       </c>
-      <c r="K53" s="7" t="n">
+      <c r="K53" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5290,7 +5309,7 @@
       <c r="J54" s="0" t="n">
         <v>0.68</v>
       </c>
-      <c r="K54" s="7" t="n">
+      <c r="K54" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5325,7 +5344,7 @@
       <c r="J55" s="0" t="n">
         <v>2.1</v>
       </c>
-      <c r="K55" s="7" t="n">
+      <c r="K55" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5360,7 +5379,7 @@
       <c r="J56" s="0" t="n">
         <v>1.76</v>
       </c>
-      <c r="K56" s="7" t="n">
+      <c r="K56" s="8" t="n">
         <v>0.26</v>
       </c>
     </row>
@@ -5395,7 +5414,7 @@
       <c r="J57" s="0" t="n">
         <v>0.05</v>
       </c>
-      <c r="K57" s="7" t="n">
+      <c r="K57" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5430,7 +5449,7 @@
       <c r="J58" s="0" t="n">
         <v>2.43</v>
       </c>
-      <c r="K58" s="7" t="n">
+      <c r="K58" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5465,7 +5484,7 @@
       <c r="J59" s="0" t="n">
         <v>0.34</v>
       </c>
-      <c r="K59" s="7" t="n">
+      <c r="K59" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5500,7 +5519,7 @@
       <c r="J60" s="0" t="n">
         <v>1.75</v>
       </c>
-      <c r="K60" s="7" t="n">
+      <c r="K60" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5535,7 +5554,7 @@
       <c r="J61" s="0" t="n">
         <v>1.44</v>
       </c>
-      <c r="K61" s="7" t="n">
+      <c r="K61" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5570,7 +5589,7 @@
       <c r="J62" s="0" t="n">
         <v>0.63</v>
       </c>
-      <c r="K62" s="7" t="n">
+      <c r="K62" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5605,7 +5624,7 @@
       <c r="J63" s="0" t="n">
         <v>2.15</v>
       </c>
-      <c r="K63" s="7" t="n">
+      <c r="K63" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5640,7 +5659,7 @@
       <c r="J64" s="0" t="n">
         <v>0.32</v>
       </c>
-      <c r="K64" s="7" t="n">
+      <c r="K64" s="8" t="n">
         <v>0.38</v>
       </c>
     </row>
@@ -5675,7 +5694,7 @@
       <c r="J65" s="0" t="n">
         <v>1.65</v>
       </c>
-      <c r="K65" s="7" t="n">
+      <c r="K65" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5710,7 +5729,7 @@
       <c r="J66" s="0" t="n">
         <v>0.46</v>
       </c>
-      <c r="K66" s="7" t="n">
+      <c r="K66" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5745,7 +5764,7 @@
       <c r="J67" s="0" t="n">
         <v>1.16</v>
       </c>
-      <c r="K67" s="7" t="n">
+      <c r="K67" s="8" t="n">
         <v>0.34</v>
       </c>
     </row>
@@ -5780,7 +5799,7 @@
       <c r="J68" s="0" t="n">
         <v>1.77</v>
       </c>
-      <c r="K68" s="7" t="n">
+      <c r="K68" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5815,7 +5834,7 @@
       <c r="J69" s="0" t="n">
         <v>1.91</v>
       </c>
-      <c r="K69" s="7" t="n">
+      <c r="K69" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5850,7 +5869,7 @@
       <c r="J70" s="0" t="n">
         <v>0.64</v>
       </c>
-      <c r="K70" s="7" t="n">
+      <c r="K70" s="8" t="n">
         <v>0.36</v>
       </c>
     </row>
@@ -5885,7 +5904,7 @@
       <c r="J71" s="0" t="n">
         <v>0.81</v>
       </c>
-      <c r="K71" s="7" t="n">
+      <c r="K71" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6864,7 +6883,7 @@
   <dimension ref="A1:Q74"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6879,8 +6898,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="9" width="8.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="11" width="8.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.53"/>
   </cols>
   <sheetData>
@@ -6915,7 +6934,7 @@
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="12" t="s">
         <v>9</v>
       </c>
       <c r="L1" s="4" t="s">
@@ -6929,7 +6948,7 @@
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="n">
+      <c r="B2" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -6957,7 +6976,7 @@
       <c r="J2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="1" t="n">
+      <c r="K2" s="12" t="n">
         <v>0.09</v>
       </c>
       <c r="L2" s="4" t="n">
@@ -6971,7 +6990,7 @@
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="n">
+      <c r="B3" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -6999,10 +7018,10 @@
       <c r="J3" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="K3" s="10" t="n">
         <v>1.22</v>
       </c>
-      <c r="L3" s="9" t="n">
+      <c r="L3" s="11" t="n">
         <v>0.95</v>
       </c>
       <c r="M3" s="1" t="s">
@@ -7013,7 +7032,7 @@
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="10" t="n">
+      <c r="B4" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -7041,10 +7060,10 @@
       <c r="J4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="K4" s="10" t="n">
         <v>0.75</v>
       </c>
-      <c r="L4" s="9" t="n">
+      <c r="L4" s="11" t="n">
         <v>0.95</v>
       </c>
       <c r="M4" s="1" t="s">
@@ -7055,7 +7074,7 @@
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="10" t="n">
+      <c r="B5" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -7083,10 +7102,10 @@
       <c r="J5" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="0" t="n">
+      <c r="K5" s="10" t="n">
         <v>1.33</v>
       </c>
-      <c r="L5" s="9" t="n">
+      <c r="L5" s="11" t="n">
         <v>1</v>
       </c>
       <c r="M5" s="1" t="s">
@@ -7097,7 +7116,7 @@
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="10" t="n">
+      <c r="B6" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -7125,10 +7144,10 @@
       <c r="J6" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="0" t="n">
+      <c r="K6" s="10" t="n">
         <v>0.6</v>
       </c>
-      <c r="L6" s="9" t="n">
+      <c r="L6" s="11" t="n">
         <v>0.9</v>
       </c>
       <c r="M6" s="1" t="s">
@@ -7139,7 +7158,7 @@
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="10" t="n">
+      <c r="B7" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -7167,10 +7186,10 @@
       <c r="J7" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="0" t="n">
+      <c r="K7" s="10" t="n">
         <v>0.79</v>
       </c>
-      <c r="L7" s="9" t="n">
+      <c r="L7" s="11" t="n">
         <v>0.9</v>
       </c>
       <c r="M7" s="1" t="s">
@@ -7181,7 +7200,7 @@
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="10" t="n">
+      <c r="B8" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -7209,10 +7228,10 @@
       <c r="J8" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="0" t="n">
+      <c r="K8" s="10" t="n">
         <v>0.08</v>
       </c>
-      <c r="L8" s="9" t="n">
+      <c r="L8" s="11" t="n">
         <v>1</v>
       </c>
       <c r="M8" s="1" t="s">
@@ -7220,10 +7239,10 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="10" t="n">
+      <c r="B9" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -7251,10 +7270,10 @@
       <c r="J9" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="0" t="n">
+      <c r="K9" s="10" t="n">
         <v>0.95</v>
       </c>
-      <c r="L9" s="11" t="n">
+      <c r="L9" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M9" s="0" t="s">
@@ -7265,7 +7284,7 @@
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="10" t="n">
+      <c r="B10" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -7293,10 +7312,10 @@
       <c r="J10" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K10" s="0" t="n">
+      <c r="K10" s="10" t="n">
         <v>1.22</v>
       </c>
-      <c r="L10" s="11" t="n">
+      <c r="L10" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M10" s="0" t="s">
@@ -7304,10 +7323,10 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="10" t="n">
+      <c r="B11" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -7335,10 +7354,10 @@
       <c r="J11" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K11" s="0" t="n">
+      <c r="K11" s="10" t="n">
         <v>0.71</v>
       </c>
-      <c r="L11" s="11" t="n">
+      <c r="L11" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M11" s="0" t="s">
@@ -7349,7 +7368,7 @@
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="10" t="n">
+      <c r="B12" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -7377,10 +7396,10 @@
       <c r="J12" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K12" s="0" t="n">
+      <c r="K12" s="10" t="n">
         <v>1.3</v>
       </c>
-      <c r="L12" s="11" t="n">
+      <c r="L12" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M12" s="0" t="s">
@@ -7388,10 +7407,10 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="7" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="10" t="n">
+      <c r="B13" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -7419,10 +7438,10 @@
       <c r="J13" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K13" s="0" t="n">
+      <c r="K13" s="10" t="n">
         <v>0.47</v>
       </c>
-      <c r="L13" s="11" t="n">
+      <c r="L13" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M13" s="0" t="s">
@@ -7430,10 +7449,10 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" s="10" t="n">
+      <c r="A14" s="7" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -7461,10 +7480,10 @@
       <c r="J14" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K14" s="0" t="n">
+      <c r="K14" s="10" t="n">
         <v>0.68</v>
       </c>
-      <c r="L14" s="11" t="n">
+      <c r="L14" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M14" s="0" t="s">
@@ -7475,7 +7494,7 @@
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="10" t="n">
+      <c r="B15" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -7503,10 +7522,10 @@
       <c r="J15" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K15" s="0" t="n">
+      <c r="K15" s="10" t="n">
         <v>1.28</v>
       </c>
-      <c r="L15" s="11" t="n">
+      <c r="L15" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M15" s="0" t="s">
@@ -7517,7 +7536,7 @@
       <c r="A16" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="10" t="n">
+      <c r="B16" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -7545,10 +7564,10 @@
       <c r="J16" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K16" s="0" t="n">
+      <c r="K16" s="10" t="n">
         <v>0.37</v>
       </c>
-      <c r="L16" s="11" t="n">
+      <c r="L16" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M16" s="0" t="s">
@@ -7559,7 +7578,7 @@
       <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="10" t="n">
+      <c r="B17" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -7587,10 +7606,10 @@
       <c r="J17" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K17" s="0" t="n">
+      <c r="K17" s="10" t="n">
         <v>0.89</v>
       </c>
-      <c r="L17" s="11" t="n">
+      <c r="L17" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M17" s="0" t="s">
@@ -7601,7 +7620,7 @@
       <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="10" t="n">
+      <c r="B18" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -7629,10 +7648,10 @@
       <c r="J18" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K18" s="0" t="n">
+      <c r="K18" s="10" t="n">
         <v>1.11</v>
       </c>
-      <c r="L18" s="11" t="n">
+      <c r="L18" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M18" s="0" t="s">
@@ -7643,7 +7662,7 @@
       <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="10" t="n">
+      <c r="B19" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -7671,10 +7690,10 @@
       <c r="J19" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K19" s="0" t="n">
+      <c r="K19" s="10" t="n">
         <v>0.9</v>
       </c>
-      <c r="L19" s="11" t="n">
+      <c r="L19" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M19" s="0" t="s">
@@ -7685,7 +7704,7 @@
       <c r="A20" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="10" t="n">
+      <c r="B20" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -7713,10 +7732,10 @@
       <c r="J20" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K20" s="0" t="n">
+      <c r="K20" s="10" t="n">
         <v>0.61</v>
       </c>
-      <c r="L20" s="11" t="n">
+      <c r="L20" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M20" s="0" t="s">
@@ -7727,7 +7746,7 @@
       <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="10" t="n">
+      <c r="B21" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -7755,10 +7774,10 @@
       <c r="J21" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K21" s="0" t="n">
+      <c r="K21" s="10" t="n">
         <v>0.16</v>
       </c>
-      <c r="L21" s="11" t="n">
+      <c r="L21" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M21" s="0" t="s">
@@ -7769,7 +7788,7 @@
       <c r="A22" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="10" t="n">
+      <c r="B22" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -7797,10 +7816,10 @@
       <c r="J22" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K22" s="0" t="n">
+      <c r="K22" s="10" t="n">
         <v>0.09</v>
       </c>
-      <c r="L22" s="11" t="n">
+      <c r="L22" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M22" s="0" t="s">
@@ -7811,7 +7830,7 @@
       <c r="A23" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="10" t="n">
+      <c r="B23" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -7839,10 +7858,10 @@
       <c r="J23" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="K23" s="0" t="n">
+      <c r="K23" s="10" t="n">
         <v>5.78</v>
       </c>
-      <c r="L23" s="11" t="n">
+      <c r="L23" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M23" s="0" t="s">
@@ -7853,7 +7872,7 @@
       <c r="A24" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="10" t="n">
+      <c r="B24" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -7881,10 +7900,10 @@
       <c r="J24" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="K24" s="0" t="n">
+      <c r="K24" s="10" t="n">
         <v>5.36</v>
       </c>
-      <c r="L24" s="11" t="n">
+      <c r="L24" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M24" s="0" t="s">
@@ -7895,7 +7914,7 @@
       <c r="A25" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="10" t="n">
+      <c r="B25" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -7923,10 +7942,10 @@
       <c r="J25" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K25" s="0" t="n">
+      <c r="K25" s="10" t="n">
         <v>2.85</v>
       </c>
-      <c r="L25" s="11" t="n">
+      <c r="L25" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M25" s="0" t="s">
@@ -7937,7 +7956,7 @@
       <c r="A26" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="10" t="n">
+      <c r="B26" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -7965,10 +7984,10 @@
       <c r="J26" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K26" s="0" t="n">
+      <c r="K26" s="10" t="n">
         <v>5.53</v>
       </c>
-      <c r="L26" s="11" t="n">
+      <c r="L26" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M26" s="0" t="s">
@@ -7979,7 +7998,7 @@
       <c r="A27" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="10" t="n">
+      <c r="B27" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8007,10 +8026,10 @@
       <c r="J27" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K27" s="0" t="n">
+      <c r="K27" s="10" t="n">
         <v>1.29</v>
       </c>
-      <c r="L27" s="11" t="n">
+      <c r="L27" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M27" s="0" t="s">
@@ -8021,7 +8040,7 @@
       <c r="A28" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="10" t="n">
+      <c r="B28" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8049,10 +8068,10 @@
       <c r="J28" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K28" s="0" t="n">
+      <c r="K28" s="10" t="n">
         <v>2.48</v>
       </c>
-      <c r="L28" s="11" t="n">
+      <c r="L28" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M28" s="0" t="s">
@@ -8063,7 +8082,7 @@
       <c r="A29" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="10" t="n">
+      <c r="B29" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8091,10 +8110,10 @@
       <c r="J29" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K29" s="0" t="n">
+      <c r="K29" s="10" t="n">
         <v>5.65</v>
       </c>
-      <c r="L29" s="11" t="n">
+      <c r="L29" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M29" s="0" t="s">
@@ -8105,7 +8124,7 @@
       <c r="A30" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="10" t="n">
+      <c r="B30" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8133,10 +8152,10 @@
       <c r="J30" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K30" s="0" t="n">
+      <c r="K30" s="10" t="n">
         <v>2.8</v>
       </c>
-      <c r="L30" s="11" t="n">
+      <c r="L30" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M30" s="0" t="s">
@@ -8147,7 +8166,7 @@
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="10" t="n">
+      <c r="B31" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8175,10 +8194,10 @@
       <c r="J31" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="K31" s="0" t="n">
+      <c r="K31" s="10" t="n">
         <v>4.32</v>
       </c>
-      <c r="L31" s="11" t="n">
+      <c r="L31" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M31" s="0" t="s">
@@ -8189,7 +8208,7 @@
       <c r="A32" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="10" t="n">
+      <c r="B32" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8217,10 +8236,10 @@
       <c r="J32" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="K32" s="0" t="n">
+      <c r="K32" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="L32" s="11" t="n">
+      <c r="L32" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M32" s="0" t="s">
@@ -8231,7 +8250,7 @@
       <c r="A33" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="10" t="n">
+      <c r="B33" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8259,10 +8278,10 @@
       <c r="J33" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K33" s="0" t="n">
+      <c r="K33" s="10" t="n">
         <v>2.53</v>
       </c>
-      <c r="L33" s="11" t="n">
+      <c r="L33" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M33" s="0" t="s">
@@ -8273,7 +8292,7 @@
       <c r="A34" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="10" t="n">
+      <c r="B34" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8301,10 +8320,10 @@
       <c r="J34" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K34" s="0" t="n">
+      <c r="K34" s="10" t="n">
         <v>4.48</v>
       </c>
-      <c r="L34" s="11" t="n">
+      <c r="L34" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M34" s="0" t="s">
@@ -8315,7 +8334,7 @@
       <c r="A35" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="10" t="n">
+      <c r="B35" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8343,10 +8362,10 @@
       <c r="J35" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="K35" s="0" t="n">
+      <c r="K35" s="10" t="n">
         <v>8.15</v>
       </c>
-      <c r="L35" s="11" t="n">
+      <c r="L35" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M35" s="0" t="s">
@@ -8357,7 +8376,7 @@
       <c r="A36" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="B36" s="10" t="n">
+      <c r="B36" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8385,10 +8404,10 @@
       <c r="J36" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K36" s="0" t="n">
+      <c r="K36" s="10" t="n">
         <v>2.97</v>
       </c>
-      <c r="L36" s="11" t="n">
+      <c r="L36" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M36" s="0" t="s">
@@ -8399,7 +8418,7 @@
       <c r="A37" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="B37" s="10" t="n">
+      <c r="B37" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8427,10 +8446,10 @@
       <c r="J37" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="K37" s="0" t="n">
+      <c r="K37" s="10" t="n">
         <v>4.3</v>
       </c>
-      <c r="L37" s="11" t="n">
+      <c r="L37" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M37" s="0" t="s">
@@ -8441,7 +8460,7 @@
       <c r="A38" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="B38" s="10" t="n">
+      <c r="B38" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8469,10 +8488,10 @@
       <c r="J38" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="K38" s="0" t="n">
+      <c r="K38" s="10" t="n">
         <v>0.41</v>
       </c>
-      <c r="L38" s="11" t="n">
+      <c r="L38" s="14" t="n">
         <v>0.53</v>
       </c>
       <c r="M38" s="0" t="s">
@@ -8483,7 +8502,7 @@
       <c r="A39" s="0" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="10" t="n">
+      <c r="B39" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8511,10 +8530,10 @@
       <c r="J39" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="K39" s="0" t="n">
+      <c r="K39" s="10" t="n">
         <v>0.16</v>
       </c>
-      <c r="L39" s="11" t="n">
+      <c r="L39" s="14" t="n">
         <v>0.66</v>
       </c>
       <c r="M39" s="0" t="s">
@@ -8525,7 +8544,7 @@
       <c r="A40" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="B40" s="10" t="n">
+      <c r="B40" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8553,10 +8572,10 @@
       <c r="J40" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="K40" s="0" t="n">
+      <c r="K40" s="10" t="n">
         <v>1.22</v>
       </c>
-      <c r="L40" s="11" t="n">
+      <c r="L40" s="14" t="n">
         <v>0.51</v>
       </c>
       <c r="M40" s="0" t="s">
@@ -8567,7 +8586,7 @@
       <c r="A41" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="B41" s="10" t="n">
+      <c r="B41" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8595,10 +8614,10 @@
       <c r="J41" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="K41" s="0" t="n">
+      <c r="K41" s="10" t="n">
         <v>0.58</v>
       </c>
-      <c r="L41" s="11" t="n">
+      <c r="L41" s="14" t="n">
         <v>0.63</v>
       </c>
       <c r="M41" s="0" t="s">
@@ -8609,7 +8628,7 @@
       <c r="A42" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="B42" s="10" t="n">
+      <c r="B42" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8637,10 +8656,10 @@
       <c r="J42" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="K42" s="0" t="n">
+      <c r="K42" s="10" t="n">
         <v>0.56</v>
       </c>
-      <c r="L42" s="11" t="n">
+      <c r="L42" s="14" t="n">
         <v>0.57</v>
       </c>
       <c r="M42" s="0" t="s">
@@ -8651,7 +8670,7 @@
       <c r="A43" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="B43" s="10" t="n">
+      <c r="B43" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8679,10 +8698,10 @@
       <c r="J43" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K43" s="0" t="n">
+      <c r="K43" s="10" t="n">
         <v>0.1</v>
       </c>
-      <c r="L43" s="11" t="n">
+      <c r="L43" s="14" t="n">
         <v>0.69</v>
       </c>
       <c r="M43" s="0" t="s">
@@ -8693,7 +8712,7 @@
       <c r="A44" s="0" t="n">
         <v>43</v>
       </c>
-      <c r="B44" s="10" t="n">
+      <c r="B44" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8721,10 +8740,10 @@
       <c r="J44" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K44" s="0" t="n">
+      <c r="K44" s="10" t="n">
         <v>1.18</v>
       </c>
-      <c r="L44" s="11" t="n">
+      <c r="L44" s="14" t="n">
         <v>0.71</v>
       </c>
       <c r="M44" s="0" t="s">
@@ -8735,7 +8754,7 @@
       <c r="A45" s="0" t="n">
         <v>44</v>
       </c>
-      <c r="B45" s="10" t="n">
+      <c r="B45" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8763,10 +8782,10 @@
       <c r="J45" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K45" s="0" t="n">
+      <c r="K45" s="10" t="n">
         <v>0.9</v>
       </c>
-      <c r="L45" s="11" t="n">
+      <c r="L45" s="14" t="n">
         <v>0.71</v>
       </c>
       <c r="M45" s="0" t="s">
@@ -8777,7 +8796,7 @@
       <c r="A46" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="B46" s="10" t="n">
+      <c r="B46" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8805,10 +8824,10 @@
       <c r="J46" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K46" s="0" t="n">
+      <c r="K46" s="10" t="n">
         <v>1.28</v>
       </c>
-      <c r="L46" s="11" t="n">
+      <c r="L46" s="14" t="n">
         <v>0.55</v>
       </c>
       <c r="M46" s="0" t="s">
@@ -8819,7 +8838,7 @@
       <c r="A47" s="0" t="n">
         <v>46</v>
       </c>
-      <c r="B47" s="10" t="n">
+      <c r="B47" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8847,10 +8866,10 @@
       <c r="J47" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K47" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L47" s="11" t="n">
+      <c r="K47" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L47" s="14" t="n">
         <v>0.55</v>
       </c>
       <c r="M47" s="0" t="s">
@@ -8861,7 +8880,7 @@
       <c r="A48" s="0" t="n">
         <v>47</v>
       </c>
-      <c r="B48" s="10" t="n">
+      <c r="B48" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8889,10 +8908,10 @@
       <c r="J48" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K48" s="0" t="n">
+      <c r="K48" s="10" t="n">
         <v>0.95</v>
       </c>
-      <c r="L48" s="11" t="n">
+      <c r="L48" s="14" t="n">
         <v>0.69</v>
       </c>
       <c r="M48" s="0" t="s">
@@ -8903,7 +8922,7 @@
       <c r="A49" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="B49" s="10" t="n">
+      <c r="B49" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -8931,10 +8950,10 @@
       <c r="J49" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K49" s="0" t="n">
+      <c r="K49" s="10" t="n">
         <v>0.95</v>
       </c>
-      <c r="L49" s="11" t="n">
+      <c r="L49" s="14" t="n">
         <v>0.69</v>
       </c>
       <c r="M49" s="0" t="s">
@@ -8945,7 +8964,7 @@
       <c r="A50" s="0" t="n">
         <v>49</v>
       </c>
-      <c r="B50" s="10" t="n">
+      <c r="B50" s="13" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8973,23 +8992,23 @@
       <c r="J50" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K50" s="0" t="n">
+      <c r="K50" s="10" t="n">
         <v>0.15</v>
       </c>
-      <c r="L50" s="11" t="n">
+      <c r="L50" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M50" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="P50" s="8"/>
-      <c r="Q50" s="7"/>
+      <c r="P50" s="9"/>
+      <c r="Q50" s="8"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="B51" s="10" t="n">
+      <c r="B51" s="13" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -9017,22 +9036,22 @@
       <c r="J51" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K51" s="0" t="n">
+      <c r="K51" s="10" t="n">
         <v>1.68</v>
       </c>
-      <c r="L51" s="11" t="n">
+      <c r="L51" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M51" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q51" s="7"/>
+      <c r="Q51" s="8"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
         <v>51</v>
       </c>
-      <c r="B52" s="10" t="n">
+      <c r="B52" s="13" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -9060,22 +9079,22 @@
       <c r="J52" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="K52" s="0" t="n">
+      <c r="K52" s="10" t="n">
         <v>1.84</v>
       </c>
-      <c r="L52" s="11" t="n">
+      <c r="L52" s="14" t="n">
         <v>0.28</v>
       </c>
       <c r="M52" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q52" s="7"/>
+      <c r="Q52" s="8"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
         <v>52</v>
       </c>
-      <c r="B53" s="10" t="n">
+      <c r="B53" s="13" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -9103,22 +9122,22 @@
       <c r="J53" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K53" s="0" t="n">
+      <c r="K53" s="10" t="n">
         <v>1.75</v>
       </c>
-      <c r="L53" s="11" t="n">
+      <c r="L53" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M53" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q53" s="7"/>
+      <c r="Q53" s="8"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
         <v>53</v>
       </c>
-      <c r="B54" s="10" t="n">
+      <c r="B54" s="13" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -9146,22 +9165,22 @@
       <c r="J54" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K54" s="0" t="n">
+      <c r="K54" s="10" t="n">
         <v>0.77</v>
       </c>
-      <c r="L54" s="11" t="n">
+      <c r="L54" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M54" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q54" s="7"/>
+      <c r="Q54" s="8"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
         <v>54</v>
       </c>
-      <c r="B55" s="10" t="n">
+      <c r="B55" s="13" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -9189,22 +9208,22 @@
       <c r="J55" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K55" s="0" t="n">
+      <c r="K55" s="10" t="n">
         <v>0.65</v>
       </c>
-      <c r="L55" s="11" t="n">
+      <c r="L55" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M55" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q55" s="7"/>
+      <c r="Q55" s="8"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="B56" s="10" t="n">
+      <c r="B56" s="13" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -9232,22 +9251,22 @@
       <c r="J56" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K56" s="0" t="n">
+      <c r="K56" s="10" t="n">
         <v>0.68</v>
       </c>
-      <c r="L56" s="11" t="n">
+      <c r="L56" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M56" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q56" s="7"/>
+      <c r="Q56" s="8"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
         <v>56</v>
       </c>
-      <c r="B57" s="10" t="n">
+      <c r="B57" s="13" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -9275,22 +9294,22 @@
       <c r="J57" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K57" s="0" t="n">
+      <c r="K57" s="10" t="n">
         <v>2.1</v>
       </c>
-      <c r="L57" s="11" t="n">
+      <c r="L57" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M57" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q57" s="7"/>
+      <c r="Q57" s="8"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
         <v>57</v>
       </c>
-      <c r="B58" s="10" t="n">
+      <c r="B58" s="13" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -9318,22 +9337,22 @@
       <c r="J58" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="K58" s="0" t="n">
+      <c r="K58" s="10" t="n">
         <v>1.76</v>
       </c>
-      <c r="L58" s="11" t="n">
+      <c r="L58" s="14" t="n">
         <v>0.26</v>
       </c>
       <c r="M58" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q58" s="7"/>
+      <c r="Q58" s="8"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
         <v>58</v>
       </c>
-      <c r="B59" s="10" t="n">
+      <c r="B59" s="13" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -9361,22 +9380,22 @@
       <c r="J59" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K59" s="0" t="n">
+      <c r="K59" s="10" t="n">
         <v>0.05</v>
       </c>
-      <c r="L59" s="11" t="n">
+      <c r="L59" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M59" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q59" s="7"/>
+      <c r="Q59" s="8"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="B60" s="10" t="n">
+      <c r="B60" s="13" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -9404,22 +9423,22 @@
       <c r="J60" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K60" s="0" t="n">
+      <c r="K60" s="10" t="n">
         <v>2.43</v>
       </c>
-      <c r="L60" s="11" t="n">
+      <c r="L60" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M60" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q60" s="7"/>
+      <c r="Q60" s="8"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="B61" s="10" t="n">
+      <c r="B61" s="13" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -9447,22 +9466,22 @@
       <c r="J61" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="K61" s="0" t="n">
+      <c r="K61" s="10" t="n">
         <v>0.34</v>
       </c>
-      <c r="L61" s="11" t="n">
+      <c r="L61" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M61" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q61" s="7"/>
+      <c r="Q61" s="8"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
         <v>61</v>
       </c>
-      <c r="B62" s="10" t="n">
+      <c r="B62" s="13" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -9490,22 +9509,22 @@
       <c r="J62" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K62" s="0" t="n">
+      <c r="K62" s="10" t="n">
         <v>1.75</v>
       </c>
-      <c r="L62" s="11" t="n">
+      <c r="L62" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M62" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q62" s="7"/>
+      <c r="Q62" s="8"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
         <v>62</v>
       </c>
-      <c r="B63" s="10" t="n">
+      <c r="B63" s="13" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -9533,22 +9552,22 @@
       <c r="J63" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K63" s="0" t="n">
+      <c r="K63" s="10" t="n">
         <v>1.75</v>
       </c>
-      <c r="L63" s="11" t="n">
+      <c r="L63" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M63" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q63" s="7"/>
+      <c r="Q63" s="8"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
         <v>63</v>
       </c>
-      <c r="B64" s="10" t="n">
+      <c r="B64" s="13" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -9576,22 +9595,22 @@
       <c r="J64" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K64" s="0" t="n">
+      <c r="K64" s="10" t="n">
         <v>1.44</v>
       </c>
-      <c r="L64" s="11" t="n">
+      <c r="L64" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M64" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q64" s="7"/>
+      <c r="Q64" s="8"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
         <v>64</v>
       </c>
-      <c r="B65" s="10" t="n">
+      <c r="B65" s="13" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -9619,22 +9638,22 @@
       <c r="J65" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K65" s="0" t="n">
+      <c r="K65" s="10" t="n">
         <v>0.63</v>
       </c>
-      <c r="L65" s="11" t="n">
+      <c r="L65" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M65" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q65" s="7"/>
+      <c r="Q65" s="8"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="B66" s="10" t="n">
+      <c r="B66" s="13" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -9662,22 +9681,22 @@
       <c r="J66" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K66" s="0" t="n">
+      <c r="K66" s="10" t="n">
         <v>2.15</v>
       </c>
-      <c r="L66" s="11" t="n">
+      <c r="L66" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M66" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Q66" s="7"/>
+      <c r="Q66" s="8"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
         <v>66</v>
       </c>
-      <c r="B67" s="10" t="n">
+      <c r="B67" s="13" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -9705,22 +9724,22 @@
       <c r="J67" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="K67" s="0" t="n">
+      <c r="K67" s="10" t="n">
         <v>0.32</v>
       </c>
-      <c r="L67" s="11" t="n">
+      <c r="L67" s="14" t="n">
         <v>0.38</v>
       </c>
       <c r="M67" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="Q67" s="7"/>
+      <c r="Q67" s="8"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
         <v>67</v>
       </c>
-      <c r="B68" s="10" t="n">
+      <c r="B68" s="13" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -9748,23 +9767,23 @@
       <c r="J68" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K68" s="0" t="n">
+      <c r="K68" s="10" t="n">
         <v>1.65</v>
       </c>
-      <c r="L68" s="11" t="n">
+      <c r="L68" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M68" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="P68" s="8"/>
-      <c r="Q68" s="7"/>
+      <c r="P68" s="9"/>
+      <c r="Q68" s="8"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
         <v>68</v>
       </c>
-      <c r="B69" s="10" t="n">
+      <c r="B69" s="13" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -9792,23 +9811,23 @@
       <c r="J69" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K69" s="0" t="n">
+      <c r="K69" s="10" t="n">
         <v>0.46</v>
       </c>
-      <c r="L69" s="11" t="n">
+      <c r="L69" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M69" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="P69" s="8"/>
-      <c r="Q69" s="7"/>
+      <c r="P69" s="9"/>
+      <c r="Q69" s="8"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
         <v>69</v>
       </c>
-      <c r="B70" s="10" t="n">
+      <c r="B70" s="13" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -9836,23 +9855,23 @@
       <c r="J70" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="K70" s="0" t="n">
+      <c r="K70" s="10" t="n">
         <v>1.16</v>
       </c>
-      <c r="L70" s="11" t="n">
+      <c r="L70" s="14" t="n">
         <v>0.34</v>
       </c>
       <c r="M70" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="P70" s="8"/>
-      <c r="Q70" s="7"/>
+      <c r="P70" s="9"/>
+      <c r="Q70" s="8"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
         <v>70</v>
       </c>
-      <c r="B71" s="10" t="n">
+      <c r="B71" s="13" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -9880,23 +9899,23 @@
       <c r="J71" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K71" s="0" t="n">
+      <c r="K71" s="10" t="n">
         <v>1.77</v>
       </c>
-      <c r="L71" s="11" t="n">
+      <c r="L71" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M71" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P71" s="8"/>
-      <c r="Q71" s="7"/>
+      <c r="P71" s="9"/>
+      <c r="Q71" s="8"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="B72" s="10" t="n">
+      <c r="B72" s="13" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -9924,23 +9943,23 @@
       <c r="J72" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K72" s="0" t="n">
+      <c r="K72" s="10" t="n">
         <v>1.91</v>
       </c>
-      <c r="L72" s="11" t="n">
+      <c r="L72" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M72" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P72" s="8"/>
-      <c r="Q72" s="7"/>
+      <c r="P72" s="9"/>
+      <c r="Q72" s="8"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
         <v>72</v>
       </c>
-      <c r="B73" s="10" t="n">
+      <c r="B73" s="13" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -9968,23 +9987,23 @@
       <c r="J73" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="K73" s="0" t="n">
+      <c r="K73" s="10" t="n">
         <v>0.64</v>
       </c>
-      <c r="L73" s="11" t="n">
+      <c r="L73" s="14" t="n">
         <v>0.36</v>
       </c>
       <c r="M73" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="P73" s="8"/>
-      <c r="Q73" s="7"/>
+      <c r="P73" s="9"/>
+      <c r="Q73" s="8"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
         <v>73</v>
       </c>
-      <c r="B74" s="10" t="n">
+      <c r="B74" s="13" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -10012,17 +10031,17 @@
       <c r="J74" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K74" s="0" t="n">
+      <c r="K74" s="10" t="n">
         <v>0.81</v>
       </c>
-      <c r="L74" s="11" t="n">
+      <c r="L74" s="14" t="n">
         <v>0</v>
       </c>
       <c r="M74" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="P74" s="8"/>
-      <c r="Q74" s="7"/>
+      <c r="P74" s="9"/>
+      <c r="Q74" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>